<commit_message>
Updated test input file for unit tests
</commit_message>
<xml_diff>
--- a/Battelle.EPA.WideAreaDecon.Model.Tests/InputFiles/ModifyParametersTest.xlsx
+++ b/Battelle.EPA.WideAreaDecon.Model.Tests/InputFiles/ModifyParametersTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERAZA\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\Battelle.EPA.WideAreaDecon.Model.Tests\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41176442-0A5C-4C99-9EBB-48EE52D04C49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5364702-85EF-4F37-B1DA-C36741017B32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="657" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="657" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -10433,8 +10433,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11401,7 +11401,7 @@
         <v>3</v>
       </c>
       <c r="G26" s="14">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
@@ -11455,8 +11455,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12127,7 +12127,7 @@
         <v>3</v>
       </c>
       <c r="G18" s="14">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
@@ -12988,8 +12988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13149,7 +13149,7 @@
       <c r="K4" s="18"/>
       <c r="L4" s="18"/>
       <c r="M4" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4" s="14">
         <v>500</v>
@@ -13186,7 +13186,7 @@
       <c r="K5" s="18"/>
       <c r="L5" s="18"/>
       <c r="M5" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" s="14">
         <v>500</v>
@@ -13223,7 +13223,7 @@
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
       <c r="M6" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" s="14">
         <v>500</v>
@@ -13260,7 +13260,7 @@
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
       <c r="M7" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" s="14">
         <v>500</v>
@@ -13297,7 +13297,7 @@
       <c r="K8" s="18"/>
       <c r="L8" s="18"/>
       <c r="M8" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="14">
         <v>500</v>
@@ -13343,7 +13343,7 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed the unit tests
</commit_message>
<xml_diff>
--- a/Battelle.EPA.WideAreaDecon.Model.Tests/InputFiles/ModifyParametersTest.xlsx
+++ b/Battelle.EPA.WideAreaDecon.Model.Tests/InputFiles/ModifyParametersTest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\Battelle.EPA.WideAreaDecon.Model.Tests\bin\Debug\netcoreapp3.1\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\Battelle.EPA.WideAreaDecon.Model.Tests\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C99B78-43D2-4D7E-A858-FFA818FA3597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D237AA-6305-484B-BE81-78141C34C43D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="657" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="326">
   <si>
     <t>SCWAD</t>
   </si>
@@ -938,9 +938,6 @@
     <t>$ / team * exit</t>
   </si>
   <si>
-    <t>Surface Area per Waste Sample</t>
-  </si>
-  <si>
     <t>Surface area that can be sampled per one waste sample</t>
   </si>
   <si>
@@ -1005,6 +1002,36 @@
   </si>
   <si>
     <t>Cost per one Waste Sample</t>
+  </si>
+  <si>
+    <t>Entry Duration Based on PPE Level (A)</t>
+  </si>
+  <si>
+    <t>Duration of each entry for one personnel donning PPE Level A</t>
+  </si>
+  <si>
+    <t>hours / entry</t>
+  </si>
+  <si>
+    <t>Entry Duration Based on PPE Level (B)</t>
+  </si>
+  <si>
+    <t>Duration of each entry for one personnel donning PPE Level B</t>
+  </si>
+  <si>
+    <t>Entry Duration Based on PPE Level (C)</t>
+  </si>
+  <si>
+    <t>Duration of each entry for one personnel donning PPE Level C</t>
+  </si>
+  <si>
+    <t>Entry Duration Based on PPE Level (D)</t>
+  </si>
+  <si>
+    <t>Duration of each entry for one personnel donning PPE Level D</t>
+  </si>
+  <si>
+    <t>Mass per Waste Sample</t>
   </si>
 </sst>
 </file>
@@ -1326,7 +1353,7 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="395">
+  <dxfs count="403">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -5182,6 +5209,20 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <i/>
         <strike/>
@@ -6244,13 +6285,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <i/>
         <strike/>
@@ -6287,34 +6321,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <i/>
         <strike/>
@@ -6333,6 +6339,41 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <i/>
         <strike/>
@@ -6344,306 +6385,6 @@
       </fill>
     </dxf>
     <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.59996337778862885"/>
@@ -6662,11 +6403,304 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -6687,41 +6721,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <i/>
         <strike/>
@@ -6751,304 +6750,46 @@
       </fill>
     </dxf>
     <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -7083,6 +6824,360 @@
       <fill>
         <patternFill>
           <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7482,24 +7577,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table156" displayName="Table156" ref="A1:O8" totalsRowShown="0" tableBorderDxfId="389">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table156" displayName="Table156" ref="A1:O8" totalsRowShown="0" tableBorderDxfId="397">
   <autoFilter ref="A1:O8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Phase" dataDxfId="388"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category" dataDxfId="387"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="386"/>
-    <tableColumn id="10" xr3:uid="{DA69379A-DE3F-42F4-AF70-91A1718AB7E0}" name="Description" dataDxfId="385"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Units" dataDxfId="384"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Distribution Type" dataDxfId="383"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parameter 1" dataDxfId="382"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Parameter 2" dataDxfId="381"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Parameter 3" dataDxfId="380"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Parameter 4" dataDxfId="379"/>
-    <tableColumn id="14" xr3:uid="{50465694-0FC6-4F52-BBDD-C2367DABB3F3}" name="Parameter 5" dataDxfId="378"/>
-    <tableColumn id="15" xr3:uid="{9D83EAB9-CB4C-4600-AF1C-4966CB714685}" name="Parameter 6" dataDxfId="377"/>
-    <tableColumn id="11" xr3:uid="{6D5D89BA-F5B6-48D7-8EB6-F84737897B28}" name="Lower Limit" dataDxfId="376"/>
-    <tableColumn id="12" xr3:uid="{48C3D1E7-422F-49D2-B091-B1AED1C3D586}" name="Upper Limit" dataDxfId="375"/>
-    <tableColumn id="13" xr3:uid="{C7F66B6D-AE49-4F19-BA50-224FF50E099F}" name="Step" dataDxfId="374"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Phase" dataDxfId="396"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category" dataDxfId="395"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="394"/>
+    <tableColumn id="10" xr3:uid="{DA69379A-DE3F-42F4-AF70-91A1718AB7E0}" name="Description" dataDxfId="393"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Units" dataDxfId="392"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Distribution Type" dataDxfId="391"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parameter 1" dataDxfId="390"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Parameter 2" dataDxfId="389"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Parameter 3" dataDxfId="388"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Parameter 4" dataDxfId="387"/>
+    <tableColumn id="14" xr3:uid="{50465694-0FC6-4F52-BBDD-C2367DABB3F3}" name="Parameter 5" dataDxfId="386"/>
+    <tableColumn id="15" xr3:uid="{9D83EAB9-CB4C-4600-AF1C-4966CB714685}" name="Parameter 6" dataDxfId="385"/>
+    <tableColumn id="11" xr3:uid="{6D5D89BA-F5B6-48D7-8EB6-F84737897B28}" name="Lower Limit" dataDxfId="384"/>
+    <tableColumn id="12" xr3:uid="{48C3D1E7-422F-49D2-B091-B1AED1C3D586}" name="Upper Limit" dataDxfId="383"/>
+    <tableColumn id="13" xr3:uid="{C7F66B6D-AE49-4F19-BA50-224FF50E099F}" name="Step" dataDxfId="382"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7722,128 +7817,128 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15" displayName="Table15" ref="A1:O29" totalsRowShown="0" tableBorderDxfId="364">
-  <autoFilter ref="A1:O29" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15" displayName="Table15" ref="A1:O33" totalsRowShown="0" tableBorderDxfId="370">
+  <autoFilter ref="A1:O33" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Phase" dataDxfId="363"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Category" dataDxfId="362"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="361"/>
-    <tableColumn id="10" xr3:uid="{8EBBFD49-190C-4C2F-A6BC-0598AAC3E788}" name="Description" dataDxfId="360"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Units" dataDxfId="359"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Distribution Type" dataDxfId="358"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Parameter 1" dataDxfId="357"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Parameter 2" dataDxfId="356"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Parameter 3" dataDxfId="355"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Parameter 4" dataDxfId="354"/>
-    <tableColumn id="14" xr3:uid="{E54D398D-B732-4333-A3F2-2EBD48BAA48B}" name="Parameter 5" dataDxfId="353"/>
-    <tableColumn id="15" xr3:uid="{47B382D4-92A3-4B8C-9C52-0458EA4788B1}" name="Parameter 6" dataDxfId="352"/>
-    <tableColumn id="11" xr3:uid="{BD4375F0-63E9-45EC-BE2E-338374C10F8B}" name="Lower Limit" dataDxfId="351"/>
-    <tableColumn id="12" xr3:uid="{E3D45A75-803F-48B4-B112-11C4C63E6D6F}" name="Upper Limit" dataDxfId="350"/>
-    <tableColumn id="13" xr3:uid="{FFEC12A7-FD01-4D8C-85CF-A25BD15B0829}" name="Step" dataDxfId="349"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Phase" dataDxfId="369"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Category" dataDxfId="368"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="367"/>
+    <tableColumn id="10" xr3:uid="{8EBBFD49-190C-4C2F-A6BC-0598AAC3E788}" name="Description" dataDxfId="366"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Units" dataDxfId="365"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Distribution Type" dataDxfId="364"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Parameter 1" dataDxfId="363"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Parameter 2" dataDxfId="362"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Parameter 3" dataDxfId="361"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Parameter 4" dataDxfId="360"/>
+    <tableColumn id="14" xr3:uid="{E54D398D-B732-4333-A3F2-2EBD48BAA48B}" name="Parameter 5" dataDxfId="359"/>
+    <tableColumn id="15" xr3:uid="{47B382D4-92A3-4B8C-9C52-0458EA4788B1}" name="Parameter 6" dataDxfId="358"/>
+    <tableColumn id="11" xr3:uid="{BD4375F0-63E9-45EC-BE2E-338374C10F8B}" name="Lower Limit" dataDxfId="357"/>
+    <tableColumn id="12" xr3:uid="{E3D45A75-803F-48B4-B112-11C4C63E6D6F}" name="Upper Limit" dataDxfId="356"/>
+    <tableColumn id="13" xr3:uid="{FFEC12A7-FD01-4D8C-85CF-A25BD15B0829}" name="Step" dataDxfId="355"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table157" displayName="Table157" ref="A1:O21" totalsRowShown="0" tableBorderDxfId="335">
-  <autoFilter ref="A1:O21" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table157" displayName="Table157" ref="A1:O25" totalsRowShown="0" tableBorderDxfId="339">
+  <autoFilter ref="A1:O25" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Phase" dataDxfId="334"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Category" dataDxfId="333"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="332"/>
-    <tableColumn id="10" xr3:uid="{2D3DA962-F373-48F5-BD94-00CC27106A46}" name="Description" dataDxfId="331"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="330"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Distribution Type" dataDxfId="329"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Parameter 1" dataDxfId="328"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Parameter 2" dataDxfId="327"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Parameter 3" dataDxfId="326"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Parameter 4" dataDxfId="325"/>
-    <tableColumn id="14" xr3:uid="{5A98E335-B701-4CC9-9D03-A85D24786F3B}" name="Parameter 5" dataDxfId="324"/>
-    <tableColumn id="15" xr3:uid="{79377D49-ED29-41CF-AC28-FD408018808C}" name="Parameter 6" dataDxfId="323"/>
-    <tableColumn id="11" xr3:uid="{FF818C38-99D8-4486-B25F-2B94B62F77AF}" name="Lower Limit" dataDxfId="322"/>
-    <tableColumn id="12" xr3:uid="{8C44E4B8-6916-4798-9055-589FE4E4C903}" name="Upper Limit" dataDxfId="321"/>
-    <tableColumn id="13" xr3:uid="{8266E46A-7EC0-42D8-91D3-D2DC1B4352DE}" name="Step" dataDxfId="320"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Phase" dataDxfId="338"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Category" dataDxfId="337"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="336"/>
+    <tableColumn id="10" xr3:uid="{2D3DA962-F373-48F5-BD94-00CC27106A46}" name="Description" dataDxfId="335"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="334"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Distribution Type" dataDxfId="333"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Parameter 1" dataDxfId="332"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Parameter 2" dataDxfId="331"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Parameter 3" dataDxfId="330"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Parameter 4" dataDxfId="329"/>
+    <tableColumn id="14" xr3:uid="{5A98E335-B701-4CC9-9D03-A85D24786F3B}" name="Parameter 5" dataDxfId="328"/>
+    <tableColumn id="15" xr3:uid="{79377D49-ED29-41CF-AC28-FD408018808C}" name="Parameter 6" dataDxfId="327"/>
+    <tableColumn id="11" xr3:uid="{FF818C38-99D8-4486-B25F-2B94B62F77AF}" name="Lower Limit" dataDxfId="326"/>
+    <tableColumn id="12" xr3:uid="{8C44E4B8-6916-4798-9055-589FE4E4C903}" name="Upper Limit" dataDxfId="325"/>
+    <tableColumn id="13" xr3:uid="{8266E46A-7EC0-42D8-91D3-D2DC1B4352DE}" name="Step" dataDxfId="324"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1579" displayName="Table1579" ref="A1:O20" totalsRowShown="0" headerRowBorderDxfId="307" tableBorderDxfId="306">
-  <autoFilter ref="A1:O20" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1579" displayName="Table1579" ref="A1:O24" totalsRowShown="0" headerRowBorderDxfId="309" tableBorderDxfId="308">
+  <autoFilter ref="A1:O24" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Phase" dataDxfId="305"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Category" dataDxfId="304"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name" dataDxfId="303"/>
-    <tableColumn id="10" xr3:uid="{A40104D1-3BF7-4068-8777-3D61F27973C1}" name="Description" dataDxfId="302"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Units" dataDxfId="301"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Distribution Type" dataDxfId="300"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Parameter 1" dataDxfId="299"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Parameter 2" dataDxfId="298"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Parameter 3" dataDxfId="297"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Parameter 4" dataDxfId="296"/>
-    <tableColumn id="14" xr3:uid="{77E616D7-C540-4C6C-A01C-31C8ADF35FBE}" name="Parameter 5" dataDxfId="295"/>
-    <tableColumn id="15" xr3:uid="{68C28D25-E41A-4D3D-A794-809A12A02364}" name="Parameter 6" dataDxfId="294"/>
-    <tableColumn id="11" xr3:uid="{83552614-5368-48EE-AE65-AA7B101E55EF}" name="Lower Limit" dataDxfId="293"/>
-    <tableColumn id="12" xr3:uid="{98998298-F4B1-4980-B79C-0BF0D0D59028}" name="Upper Limit" dataDxfId="292"/>
-    <tableColumn id="13" xr3:uid="{8E3814A1-C526-4157-B0D9-1258E47ACA45}" name="Step" dataDxfId="291"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Phase" dataDxfId="307"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Category" dataDxfId="306"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name" dataDxfId="305"/>
+    <tableColumn id="10" xr3:uid="{A40104D1-3BF7-4068-8777-3D61F27973C1}" name="Description" dataDxfId="304"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Units" dataDxfId="303"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Distribution Type" dataDxfId="302"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Parameter 1" dataDxfId="301"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Parameter 2" dataDxfId="300"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Parameter 3" dataDxfId="299"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Parameter 4" dataDxfId="298"/>
+    <tableColumn id="14" xr3:uid="{77E616D7-C540-4C6C-A01C-31C8ADF35FBE}" name="Parameter 5" dataDxfId="297"/>
+    <tableColumn id="15" xr3:uid="{68C28D25-E41A-4D3D-A794-809A12A02364}" name="Parameter 6" dataDxfId="296"/>
+    <tableColumn id="11" xr3:uid="{83552614-5368-48EE-AE65-AA7B101E55EF}" name="Lower Limit" dataDxfId="295"/>
+    <tableColumn id="12" xr3:uid="{98998298-F4B1-4980-B79C-0BF0D0D59028}" name="Upper Limit" dataDxfId="294"/>
+    <tableColumn id="13" xr3:uid="{8E3814A1-C526-4157-B0D9-1258E47ACA45}" name="Step" dataDxfId="293"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{7330A672-C943-4362-821B-755573408116}" name="Table1521" displayName="Table1521" ref="A1:O31" totalsRowShown="0" tableBorderDxfId="285">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{7330A672-C943-4362-821B-755573408116}" name="Table1521" displayName="Table1521" ref="A1:O31" totalsRowShown="0" tableBorderDxfId="287">
   <autoFilter ref="A1:O31" xr:uid="{7330A672-C943-4362-821B-755573408116}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{B133B9E4-820A-4680-BCDD-704A3C728372}" name="Phase" dataDxfId="284"/>
-    <tableColumn id="1" xr3:uid="{0C52E358-F746-4AB6-A186-E9F57DC3488C}" name="Category" dataDxfId="283"/>
-    <tableColumn id="2" xr3:uid="{3EB687B2-94CD-4468-838E-53D1ED3E92AD}" name="Name" dataDxfId="282"/>
-    <tableColumn id="10" xr3:uid="{48F735C1-6CD8-47D1-8F20-910C557D8DE5}" name="Description" dataDxfId="281"/>
-    <tableColumn id="3" xr3:uid="{D0BD7EC3-8CC3-442D-B9BD-BE7C714173ED}" name="Units" dataDxfId="280"/>
-    <tableColumn id="4" xr3:uid="{3AA698E5-4D28-4598-A0BE-C99F25507CDF}" name="Distribution Type" dataDxfId="279"/>
-    <tableColumn id="5" xr3:uid="{25A9745D-9B26-408E-A43E-16235B7DFC6C}" name="Parameter 1" dataDxfId="278"/>
-    <tableColumn id="6" xr3:uid="{CA609044-DDDF-4C5D-9F10-C588B31C94B0}" name="Parameter 2" dataDxfId="277"/>
-    <tableColumn id="7" xr3:uid="{CCB86206-76D0-4ABB-A2F9-AE89D61B8D45}" name="Parameter 3" dataDxfId="276"/>
-    <tableColumn id="8" xr3:uid="{9DDAD0C7-7150-4C7A-8CC1-7CA55268D2F2}" name="Parameter 4" dataDxfId="275"/>
-    <tableColumn id="14" xr3:uid="{C33C5E5C-1FFC-4C5F-9F33-FD7D79906B77}" name="Parameter 5" dataDxfId="274"/>
-    <tableColumn id="15" xr3:uid="{4EC6D868-8CE7-424C-9953-B01CAA077D51}" name="Parameter 6" dataDxfId="273"/>
-    <tableColumn id="11" xr3:uid="{C8797205-E1CA-4AD8-BE1C-EBCFC768BE51}" name="Lower Limit" dataDxfId="272"/>
-    <tableColumn id="12" xr3:uid="{2E665777-FC21-4123-AC7B-1763610C7AF4}" name="Upper Limit" dataDxfId="271"/>
-    <tableColumn id="13" xr3:uid="{0283BE4B-5056-4073-98BD-609D701ACEA2}" name="Step" dataDxfId="270"/>
+    <tableColumn id="9" xr3:uid="{B133B9E4-820A-4680-BCDD-704A3C728372}" name="Phase" dataDxfId="286"/>
+    <tableColumn id="1" xr3:uid="{0C52E358-F746-4AB6-A186-E9F57DC3488C}" name="Category" dataDxfId="285"/>
+    <tableColumn id="2" xr3:uid="{3EB687B2-94CD-4468-838E-53D1ED3E92AD}" name="Name" dataDxfId="284"/>
+    <tableColumn id="10" xr3:uid="{48F735C1-6CD8-47D1-8F20-910C557D8DE5}" name="Description" dataDxfId="283"/>
+    <tableColumn id="3" xr3:uid="{D0BD7EC3-8CC3-442D-B9BD-BE7C714173ED}" name="Units" dataDxfId="282"/>
+    <tableColumn id="4" xr3:uid="{3AA698E5-4D28-4598-A0BE-C99F25507CDF}" name="Distribution Type" dataDxfId="281"/>
+    <tableColumn id="5" xr3:uid="{25A9745D-9B26-408E-A43E-16235B7DFC6C}" name="Parameter 1" dataDxfId="280"/>
+    <tableColumn id="6" xr3:uid="{CA609044-DDDF-4C5D-9F10-C588B31C94B0}" name="Parameter 2" dataDxfId="279"/>
+    <tableColumn id="7" xr3:uid="{CCB86206-76D0-4ABB-A2F9-AE89D61B8D45}" name="Parameter 3" dataDxfId="278"/>
+    <tableColumn id="8" xr3:uid="{9DDAD0C7-7150-4C7A-8CC1-7CA55268D2F2}" name="Parameter 4" dataDxfId="277"/>
+    <tableColumn id="14" xr3:uid="{C33C5E5C-1FFC-4C5F-9F33-FD7D79906B77}" name="Parameter 5" dataDxfId="276"/>
+    <tableColumn id="15" xr3:uid="{4EC6D868-8CE7-424C-9953-B01CAA077D51}" name="Parameter 6" dataDxfId="275"/>
+    <tableColumn id="11" xr3:uid="{C8797205-E1CA-4AD8-BE1C-EBCFC768BE51}" name="Lower Limit" dataDxfId="274"/>
+    <tableColumn id="12" xr3:uid="{2E665777-FC21-4123-AC7B-1763610C7AF4}" name="Upper Limit" dataDxfId="273"/>
+    <tableColumn id="13" xr3:uid="{0283BE4B-5056-4073-98BD-609D701ACEA2}" name="Step" dataDxfId="272"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table15793" displayName="Table15793" ref="A1:O8" totalsRowShown="0" headerRowBorderDxfId="265" tableBorderDxfId="264">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table15793" displayName="Table15793" ref="A1:O8" totalsRowShown="0" headerRowBorderDxfId="267" tableBorderDxfId="266">
   <autoFilter ref="A1:O8" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Phase" dataDxfId="263"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Category" dataDxfId="262"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Name" dataDxfId="261"/>
-    <tableColumn id="10" xr3:uid="{4482773E-AA48-4795-9A9F-10283D12A976}" name="Description" dataDxfId="260"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Units" dataDxfId="259"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Distribution Type" dataDxfId="258"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Parameter 1" dataDxfId="257"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Parameter 2" dataDxfId="256"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Parameter 3" dataDxfId="255"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Parameter 4" dataDxfId="254"/>
-    <tableColumn id="14" xr3:uid="{41E058E9-8EB6-430E-BC58-82195628B7D1}" name="Parameter 5" dataDxfId="253"/>
-    <tableColumn id="15" xr3:uid="{1CA16974-E252-4655-813D-3FC48E8CCF45}" name="Parameter 6" dataDxfId="252"/>
-    <tableColumn id="11" xr3:uid="{0ED7EC4B-FD74-44E3-B1E6-428C431FDA88}" name="Lower Limit" dataDxfId="251"/>
-    <tableColumn id="12" xr3:uid="{4CA3754D-692A-40C0-BCC5-14D0E3AAF144}" name="Upper Limit" dataDxfId="250"/>
-    <tableColumn id="13" xr3:uid="{D4791B88-6435-44AE-9946-77D4E8CB6EA8}" name="Step" dataDxfId="249"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Phase" dataDxfId="265"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Category" dataDxfId="264"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Name" dataDxfId="263"/>
+    <tableColumn id="10" xr3:uid="{4482773E-AA48-4795-9A9F-10283D12A976}" name="Description" dataDxfId="262"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Units" dataDxfId="261"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Distribution Type" dataDxfId="260"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Parameter 1" dataDxfId="259"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Parameter 2" dataDxfId="258"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Parameter 3" dataDxfId="257"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Parameter 4" dataDxfId="256"/>
+    <tableColumn id="14" xr3:uid="{41E058E9-8EB6-430E-BC58-82195628B7D1}" name="Parameter 5" dataDxfId="255"/>
+    <tableColumn id="15" xr3:uid="{1CA16974-E252-4655-813D-3FC48E8CCF45}" name="Parameter 6" dataDxfId="254"/>
+    <tableColumn id="11" xr3:uid="{0ED7EC4B-FD74-44E3-B1E6-428C431FDA88}" name="Lower Limit" dataDxfId="253"/>
+    <tableColumn id="12" xr3:uid="{4CA3754D-692A-40C0-BCC5-14D0E3AAF144}" name="Upper Limit" dataDxfId="252"/>
+    <tableColumn id="13" xr3:uid="{D4791B88-6435-44AE-9946-77D4E8CB6EA8}" name="Step" dataDxfId="251"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157910" displayName="Table157910" ref="A1:O28" totalsRowShown="0" headerRowBorderDxfId="240" tableBorderDxfId="239">
-  <autoFilter ref="A1:O28" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157910" displayName="Table157910" ref="A1:O30" totalsRowShown="0" headerRowBorderDxfId="240" tableBorderDxfId="239">
+  <autoFilter ref="A1:O30" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J2">
     <sortCondition ref="B1:B2"/>
   </sortState>
@@ -8238,10 +8333,10 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8452,22 +8547,22 @@
         <v>126</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>219</v>
+        <v>312</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>166</v>
+        <v>313</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="11">
-        <v>150</v>
+        <v>254.19</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
@@ -8475,10 +8570,10 @@
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
       <c r="M6" s="11">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="N6" s="11">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="O6" s="11">
         <v>0.1</v>
@@ -8489,22 +8584,22 @@
         <v>126</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>69</v>
+        <v>314</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>167</v>
+        <v>315</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="11">
-        <v>250</v>
+        <v>19</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
@@ -8512,10 +8607,10 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="11">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="N7" s="11">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="O7" s="11">
         <v>0.1</v>
@@ -8529,10 +8624,10 @@
         <v>29</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>64</v>
@@ -8541,7 +8636,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="11">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
@@ -8549,10 +8644,10 @@
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
       <c r="M8" s="11">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="N8" s="11">
-        <v>105</v>
+        <v>200</v>
       </c>
       <c r="O8" s="11">
         <v>0.1</v>
@@ -8563,22 +8658,22 @@
         <v>126</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>221</v>
+        <v>69</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G9" s="11">
-        <v>110</v>
+        <v>250</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
@@ -8586,10 +8681,10 @@
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
       <c r="M9" s="11">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="N9" s="11">
-        <v>125</v>
+        <v>500</v>
       </c>
       <c r="O9" s="11">
         <v>0.1</v>
@@ -8603,10 +8698,10 @@
         <v>29</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>64</v>
@@ -8615,7 +8710,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="11">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
@@ -8623,10 +8718,10 @@
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
       <c r="M10" s="11">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="N10" s="11">
-        <v>170</v>
+        <v>105</v>
       </c>
       <c r="O10" s="11">
         <v>0.1</v>
@@ -8637,22 +8732,22 @@
         <v>126</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>313</v>
+        <v>221</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>314</v>
+        <v>160</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G11" s="11">
-        <v>520</v>
+        <v>110</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
@@ -8663,7 +8758,7 @@
         <v>100</v>
       </c>
       <c r="N11" s="11">
-        <v>600</v>
+        <v>125</v>
       </c>
       <c r="O11" s="11">
         <v>0.1</v>
@@ -8674,22 +8769,22 @@
         <v>126</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>315</v>
+        <v>222</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>316</v>
+        <v>161</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G12" s="11">
-        <v>19</v>
+        <v>130</v>
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
@@ -8697,10 +8792,10 @@
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
       <c r="M12" s="11">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="N12" s="11">
-        <v>50</v>
+        <v>170</v>
       </c>
       <c r="O12" s="11">
         <v>0.1</v>
@@ -8711,22 +8806,22 @@
         <v>126</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>223</v>
+        <v>312</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>162</v>
+        <v>313</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G13" s="11">
-        <v>190</v>
+        <v>520</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
@@ -8734,10 +8829,10 @@
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
       <c r="M13" s="11">
-        <v>165</v>
+        <v>100</v>
       </c>
       <c r="N13" s="11">
-        <v>250</v>
+        <v>600</v>
       </c>
       <c r="O13" s="11">
         <v>0.1</v>
@@ -8751,19 +8846,19 @@
         <v>45</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>248</v>
+        <v>314</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>168</v>
+        <v>315</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G14" s="11">
-        <v>235.42</v>
+        <v>19</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
@@ -8771,10 +8866,10 @@
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
       <c r="M14" s="11">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="N14" s="11">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="O14" s="11">
         <v>0.1</v>
@@ -8785,22 +8880,22 @@
         <v>126</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>70</v>
+        <v>223</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G15" s="11">
-        <v>238</v>
+        <v>190</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
@@ -8808,10 +8903,10 @@
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
       <c r="M15" s="11">
-        <v>100</v>
+        <v>165</v>
       </c>
       <c r="N15" s="11">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="O15" s="11">
         <v>0.1</v>
@@ -8825,19 +8920,19 @@
         <v>45</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G16" s="11">
-        <v>19</v>
+        <v>235.42</v>
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
@@ -8845,10 +8940,10 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
       <c r="M16" s="11">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="N16" s="11">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="O16" s="11">
         <v>0.1</v>
@@ -8859,22 +8954,22 @@
         <v>126</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>244</v>
+        <v>70</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>196</v>
+        <v>66</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G17" s="11">
-        <v>1.53612754751869</v>
+        <v>238</v>
       </c>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
@@ -8882,36 +8977,36 @@
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
       <c r="M17" s="11">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N17" s="11">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="O17" s="11">
         <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>288</v>
+        <v>249</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>289</v>
+        <v>170</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>290</v>
+        <v>66</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="11">
-        <v>252</v>
+        <v>19</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
@@ -8919,36 +9014,36 @@
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
       <c r="M18" s="11">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N18" s="11">
-        <v>1000</v>
+        <v>30</v>
       </c>
       <c r="O18" s="11">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>291</v>
+        <v>244</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>292</v>
+        <v>195</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>293</v>
+        <v>196</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G19" s="11">
-        <v>697</v>
+        <v>1.53612754751869</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
@@ -8959,33 +9054,33 @@
         <v>0</v>
       </c>
       <c r="N19" s="11">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="O19" s="11">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="10" t="s">
         <v>126</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>71</v>
+        <v>288</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>171</v>
+        <v>289</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>66</v>
+        <v>290</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G20" s="11">
-        <v>391.59</v>
+        <v>252</v>
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
@@ -8993,36 +9088,36 @@
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
       <c r="M20" s="11">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="N20" s="11">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="O20" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="10" t="s">
         <v>126</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>72</v>
+        <v>291</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>172</v>
+        <v>292</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>66</v>
+        <v>293</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G21" s="11">
-        <v>144.83000000000001</v>
+        <v>697</v>
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
@@ -9030,10 +9125,10 @@
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
       <c r="M21" s="11">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="N21" s="11">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="O21" s="11">
         <v>1</v>
@@ -9047,10 +9142,10 @@
         <v>42</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>66</v>
@@ -9059,7 +9154,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="11">
-        <v>66.599999999999994</v>
+        <v>391.59</v>
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
@@ -9067,10 +9162,10 @@
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
       <c r="M22" s="11">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="N22" s="11">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="O22" s="11">
         <v>1</v>
@@ -9084,10 +9179,10 @@
         <v>42</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>66</v>
@@ -9096,7 +9191,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="11">
-        <v>64.319999999999993</v>
+        <v>144.83000000000001</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
@@ -9104,10 +9199,10 @@
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
       <c r="M23" s="11">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N23" s="11">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="O23" s="11">
         <v>1</v>
@@ -9118,22 +9213,22 @@
         <v>126</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>247</v>
+        <v>73</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F24" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G24" s="11">
-        <v>1007.082</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
@@ -9141,10 +9236,10 @@
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
       <c r="M24" s="11">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="N24" s="11">
-        <v>1500</v>
+        <v>100</v>
       </c>
       <c r="O24" s="11">
         <v>1</v>
@@ -9154,97 +9249,97 @@
       <c r="A25" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B25" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>75</v>
+      <c r="B25" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G25" s="14">
-        <v>520</v>
-      </c>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="14">
-        <v>200</v>
-      </c>
-      <c r="N25" s="14">
-        <v>800</v>
-      </c>
-      <c r="O25" s="14">
+      <c r="G25" s="11">
+        <v>64.319999999999993</v>
+      </c>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="11">
+        <v>0</v>
+      </c>
+      <c r="N25" s="11">
+        <v>100</v>
+      </c>
+      <c r="O25" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B26" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="E26" s="14" t="s">
+      <c r="B26" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>68</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G26" s="14">
-        <v>225</v>
-      </c>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="14">
-        <v>0</v>
-      </c>
-      <c r="N26" s="14">
+      <c r="G26" s="11">
+        <v>1007.082</v>
+      </c>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="11">
         <v>500</v>
       </c>
-      <c r="O26" s="14">
-        <v>0.1</v>
+      <c r="N26" s="11">
+        <v>1500</v>
+      </c>
+      <c r="O26" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>263</v>
+        <v>176</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>264</v>
+        <v>75</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G27" s="14">
-        <v>0.1</v>
+        <v>520</v>
       </c>
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
@@ -9252,13 +9347,13 @@
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
       <c r="M27" s="14">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N27" s="14">
-        <v>10</v>
+        <v>800</v>
       </c>
       <c r="O27" s="14">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -9269,19 +9364,19 @@
         <v>32</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>235</v>
+        <v>199</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>234</v>
+        <v>68</v>
       </c>
       <c r="F28" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G28" s="14">
-        <v>350</v>
+        <v>225</v>
       </c>
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
@@ -9295,51 +9390,135 @@
         <v>500</v>
       </c>
       <c r="O28" s="14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="14">
+        <v>0</v>
+      </c>
+      <c r="N29" s="14">
+        <v>10</v>
+      </c>
+      <c r="O29" s="14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="14">
+        <v>350</v>
+      </c>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="14">
+        <v>0</v>
+      </c>
+      <c r="N30" s="14">
+        <v>500</v>
+      </c>
+      <c r="O30" s="14">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G2:L10 G13:L28">
-    <cfRule type="expression" dxfId="248" priority="34">
+  <conditionalFormatting sqref="G2:L5 G8:L30">
+    <cfRule type="expression" dxfId="250" priority="38">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="247" priority="6">
+    <cfRule type="expression" dxfId="249" priority="10">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="246" priority="7">
+    <cfRule type="expression" dxfId="248" priority="11">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:L2 A3:L10 F20:F28 G20:L25 A20:E25 A13:L17">
-    <cfRule type="expression" dxfId="245" priority="133">
+  <conditionalFormatting sqref="B2:L2 A3:L5 F22:F30 G22:L27 A22:E27 A15:L19 A8:L12">
+    <cfRule type="expression" dxfId="247" priority="137">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11:L11">
-    <cfRule type="expression" dxfId="244" priority="4">
-      <formula>NOT((COLUMN(G11)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F11, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+  <conditionalFormatting sqref="A13:L13">
+    <cfRule type="expression" dxfId="246" priority="7">
+      <formula>ISBLANK($F13)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:L11">
-    <cfRule type="expression" dxfId="243" priority="3">
-      <formula>ISBLANK($F11)</formula>
+  <conditionalFormatting sqref="A14:L14">
+    <cfRule type="expression" dxfId="245" priority="6">
+      <formula>ISBLANK($F14)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G12:L12">
-    <cfRule type="expression" dxfId="242" priority="1">
-      <formula>NOT((COLUMN(G12)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F12, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+  <conditionalFormatting sqref="G6:L6">
+    <cfRule type="expression" dxfId="244" priority="4">
+      <formula>NOT((COLUMN(G6)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F6, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12:L12">
+  <conditionalFormatting sqref="A6:L6">
+    <cfRule type="expression" dxfId="243" priority="3">
+      <formula>ISBLANK($F6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7:L7">
+    <cfRule type="expression" dxfId="242" priority="1">
+      <formula>NOT((COLUMN(G7)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F7, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:L7">
     <cfRule type="expression" dxfId="241" priority="2">
-      <formula>ISBLANK($F12)</formula>
+      <formula>ISBLANK($F7)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F32" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F34" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>
@@ -12163,25 +12342,25 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A2:L2 A8:L8 F3:L6 D3:D6 A3:B7">
-    <cfRule type="expression" dxfId="394" priority="138">
+    <cfRule type="expression" dxfId="402" priority="138">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="393" priority="139">
+    <cfRule type="expression" dxfId="401" priority="139">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C6 E3:E6">
-    <cfRule type="expression" dxfId="392" priority="5">
+    <cfRule type="expression" dxfId="400" priority="5">
       <formula>ISBLANK($F3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:L7">
-    <cfRule type="expression" dxfId="391" priority="1">
+    <cfRule type="expression" dxfId="399" priority="1">
       <formula>NOT((COLUMN(G7)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F7, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:L7">
-    <cfRule type="expression" dxfId="390" priority="2">
+    <cfRule type="expression" dxfId="398" priority="2">
       <formula>ISBLANK($F7)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12201,10 +12380,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:O21"/>
+    <sheetView topLeftCell="D8" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13077,7 +13256,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>126</v>
       </c>
@@ -13114,152 +13293,152 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="13" t="s">
+    <row r="25" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>254</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>224</v>
+      <c r="B25" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>318</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G25" s="14">
+        <v>1</v>
+      </c>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="11">
         <v>0</v>
       </c>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="14">
-        <v>0</v>
-      </c>
-      <c r="N25" s="14">
-        <v>1</v>
-      </c>
-      <c r="O25" s="14">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
+      <c r="N25" s="11">
+        <v>5</v>
+      </c>
+      <c r="O25" s="11">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B26" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>259</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>224</v>
+      <c r="B26" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>318</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G26" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="11">
         <v>0</v>
       </c>
-      <c r="N26" s="14">
-        <v>1</v>
-      </c>
-      <c r="O26" s="14">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
+      <c r="N26" s="11">
+        <v>5</v>
+      </c>
+      <c r="O26" s="11">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>224</v>
+      <c r="B27" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>318</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G27" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="14">
+        <v>2</v>
+      </c>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="11">
         <v>0</v>
       </c>
-      <c r="N27" s="14">
-        <v>1</v>
-      </c>
-      <c r="O27" s="14">
-        <v>1E-3</v>
+      <c r="N27" s="11">
+        <v>5</v>
+      </c>
+      <c r="O27" s="11">
+        <v>0.01</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>224</v>
+      <c r="B28" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>318</v>
       </c>
       <c r="F28" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G28" s="14">
+        <v>2.5</v>
+      </c>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="11">
         <v>0</v>
       </c>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="14">
-        <v>0</v>
-      </c>
-      <c r="N28" s="14">
-        <v>1</v>
-      </c>
-      <c r="O28" s="14">
-        <v>1E-3</v>
+      <c r="N28" s="11">
+        <v>5</v>
+      </c>
+      <c r="O28" s="11">
+        <v>0.01</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -13267,13 +13446,13 @@
         <v>126</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>237</v>
+        <v>258</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>224</v>
@@ -13282,7 +13461,7 @@
         <v>3</v>
       </c>
       <c r="G29" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
@@ -13296,54 +13475,212 @@
         <v>1</v>
       </c>
       <c r="O29" s="14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="14">
+        <v>0</v>
+      </c>
+      <c r="N30" s="14">
+        <v>1</v>
+      </c>
+      <c r="O30" s="14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="14">
+        <v>0</v>
+      </c>
+      <c r="N31" s="14">
+        <v>1</v>
+      </c>
+      <c r="O31" s="14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="14">
+        <v>0</v>
+      </c>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="14">
+        <v>0</v>
+      </c>
+      <c r="N32" s="14">
+        <v>1</v>
+      </c>
+      <c r="O32" s="14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" s="14">
+        <v>1</v>
+      </c>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="14">
+        <v>0</v>
+      </c>
+      <c r="N33" s="14">
+        <v>1</v>
+      </c>
+      <c r="O33" s="14">
         <v>0.01</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G2:L19 G22:L29">
-    <cfRule type="expression" dxfId="373" priority="63">
+  <conditionalFormatting sqref="G2:L24 G29:L33">
+    <cfRule type="expression" dxfId="381" priority="68">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D19 D13 A2:A17 D3:D6 A19 A18:B18 A22:A29">
-    <cfRule type="expression" dxfId="372" priority="47">
+  <conditionalFormatting sqref="D19 D13 A2:A17 D3:D6 A18:B18 A19:A24 A29:A33">
+    <cfRule type="expression" dxfId="380" priority="52">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="371" priority="48">
+    <cfRule type="expression" dxfId="379" priority="53">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:L2 B22:E22 B19:C19 B7:E12 B13:C13 E13 B3:C6 E3:L4 B14:E17 E5:E6 F5:L17 E19:L19 G22:L22 F22:F29">
-    <cfRule type="expression" dxfId="370" priority="146">
+  <conditionalFormatting sqref="B2:L2 B22:E22 B19:C19 B7:E12 B13:C13 E13 B3:C6 E3:L4 B14:E17 E5:E6 F5:L17 E19:L19 G22:L22 F22:F24 F29:F33">
+    <cfRule type="expression" dxfId="378" priority="151">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:L18">
-    <cfRule type="expression" dxfId="369" priority="6">
+    <cfRule type="expression" dxfId="377" priority="11">
       <formula>ISBLANK($F18)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20:L21">
-    <cfRule type="expression" dxfId="368" priority="3">
-      <formula>NOT((COLUMN(G20)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F20, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20:A21">
-    <cfRule type="expression" dxfId="367" priority="1">
-      <formula>ISBLANK($F20)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="366" priority="2">
-      <formula>NOT((COLUMN(A20)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F20, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F20:F21">
-    <cfRule type="expression" dxfId="365" priority="4">
+    <cfRule type="expression" dxfId="376" priority="9">
       <formula>ISBLANK($F20)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H25:L28">
+    <cfRule type="expression" dxfId="375" priority="4">
+      <formula>NOT((COLUMN(H25)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F25, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25:A28 D25:D28">
+    <cfRule type="expression" dxfId="374" priority="2">
+      <formula>ISBLANK($F25)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="373" priority="3">
+      <formula>NOT((COLUMN(A25)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F25, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25:C28 E25:F28 H25:L28">
+    <cfRule type="expression" dxfId="372" priority="5">
+      <formula>ISBLANK($F25)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G25:G28">
+    <cfRule type="expression" dxfId="371" priority="1">
+      <formula>NOT((COLUMN(G25)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F25, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F29" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F33" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>
@@ -13357,10 +13694,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="G17" sqref="G17:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13937,7 +14274,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>126</v>
       </c>
@@ -13974,152 +14311,152 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>254</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>224</v>
+      <c r="B17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>318</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G17" s="14">
+        <v>1</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="11">
         <v>0</v>
       </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="14">
-        <v>0</v>
-      </c>
-      <c r="N17" s="14">
-        <v>1</v>
-      </c>
-      <c r="O17" s="14">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
+      <c r="N17" s="11">
+        <v>5</v>
+      </c>
+      <c r="O17" s="11">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>259</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>224</v>
+      <c r="B18" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>318</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="11">
         <v>0</v>
       </c>
-      <c r="N18" s="14">
-        <v>1</v>
-      </c>
-      <c r="O18" s="14">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
+      <c r="N18" s="11">
+        <v>5</v>
+      </c>
+      <c r="O18" s="11">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>224</v>
+      <c r="B19" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>318</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G19" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="14">
+        <v>2</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="11">
         <v>0</v>
       </c>
-      <c r="N19" s="14">
-        <v>1</v>
-      </c>
-      <c r="O19" s="14">
-        <v>1E-3</v>
+      <c r="N19" s="11">
+        <v>5</v>
+      </c>
+      <c r="O19" s="11">
+        <v>0.01</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>224</v>
+      <c r="B20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>318</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G20" s="14">
+        <v>2.5</v>
+      </c>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="11">
         <v>0</v>
       </c>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="14">
-        <v>0</v>
-      </c>
-      <c r="N20" s="14">
-        <v>1</v>
-      </c>
-      <c r="O20" s="14">
-        <v>1E-3</v>
+      <c r="N20" s="11">
+        <v>5</v>
+      </c>
+      <c r="O20" s="11">
+        <v>0.01</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -14127,13 +14464,13 @@
         <v>126</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>239</v>
+        <v>258</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>224</v>
@@ -14142,7 +14479,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
@@ -14156,74 +14493,232 @@
         <v>1</v>
       </c>
       <c r="O21" s="14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="14">
+        <v>0</v>
+      </c>
+      <c r="N22" s="14">
+        <v>1</v>
+      </c>
+      <c r="O22" s="14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="14">
+        <v>0</v>
+      </c>
+      <c r="N23" s="14">
+        <v>1</v>
+      </c>
+      <c r="O23" s="14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="14">
+        <v>0</v>
+      </c>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="14">
+        <v>0</v>
+      </c>
+      <c r="N24" s="14">
+        <v>1</v>
+      </c>
+      <c r="O24" s="14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="14">
+        <v>1</v>
+      </c>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="14">
+        <v>0</v>
+      </c>
+      <c r="N25" s="14">
+        <v>1</v>
+      </c>
+      <c r="O25" s="14">
         <v>0.01</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G2:L13 G16:L21">
-    <cfRule type="expression" dxfId="348" priority="60">
+  <conditionalFormatting sqref="G2:L16 G21:L25">
+    <cfRule type="expression" dxfId="354" priority="66">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13 D9 D3:D6 A2:A11 A13 A12:B12 A16:A21">
-    <cfRule type="expression" dxfId="347" priority="41">
+  <conditionalFormatting sqref="D13 D9 D3:D6 A2:A11 A12:B12 A13:A16 A21:A25">
+    <cfRule type="expression" dxfId="353" priority="47">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="346" priority="42">
+    <cfRule type="expression" dxfId="352" priority="48">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:E16 B7:E7 B8:C11 E8:E11 B2:C6 E2:L4 E5:E6 F5:L11 E13:L13 B13:C13 G16:L16 F16:F21">
-    <cfRule type="expression" dxfId="345" priority="151">
+  <conditionalFormatting sqref="B7:E7 B8:C11 E8:E11 B2:C6 E2:L4 E5:E6 F5:L11 E13:L13 B13:C13 B16:L16 F21:F25">
+    <cfRule type="expression" dxfId="351" priority="157">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="344" priority="14">
+    <cfRule type="expression" dxfId="350" priority="20">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="expression" dxfId="343" priority="13">
+    <cfRule type="expression" dxfId="349" priority="19">
       <formula>ISBLANK($F8)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="342" priority="12">
+    <cfRule type="expression" dxfId="348" priority="18">
       <formula>ISBLANK($F11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="341" priority="11">
+    <cfRule type="expression" dxfId="347" priority="17">
       <formula>ISBLANK($F10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:L12">
-    <cfRule type="expression" dxfId="340" priority="6">
+    <cfRule type="expression" dxfId="346" priority="12">
       <formula>ISBLANK($F12)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G14:L15">
-    <cfRule type="expression" dxfId="339" priority="3">
-      <formula>NOT((COLUMN(G14)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F14, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:A15">
-    <cfRule type="expression" dxfId="338" priority="1">
-      <formula>ISBLANK($F14)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="337" priority="2">
-      <formula>NOT((COLUMN(A14)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F14, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F14:F15">
-    <cfRule type="expression" dxfId="336" priority="4">
+    <cfRule type="expression" dxfId="345" priority="10">
       <formula>ISBLANK($F14)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H17:L20">
+    <cfRule type="expression" dxfId="344" priority="5">
+      <formula>NOT((COLUMN(H17)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F17, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17:A20 D17:D20">
+    <cfRule type="expression" dxfId="343" priority="3">
+      <formula>ISBLANK($F17)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="342" priority="4">
+      <formula>NOT((COLUMN(A17)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F17, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:C20 E17:F20 H17:L20">
+    <cfRule type="expression" dxfId="341" priority="6">
+      <formula>ISBLANK($F17)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17:G20">
+    <cfRule type="expression" dxfId="340" priority="1">
+      <formula>NOT((COLUMN(G17)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F17, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F22" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F26" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>
@@ -14237,10 +14732,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G17" sqref="G17:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14816,7 +15311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>126</v>
       </c>
@@ -14853,214 +15348,372 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>254</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>224</v>
+      <c r="B17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>318</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G17" s="14">
+        <v>1</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="11">
         <v>0</v>
       </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="14">
-        <v>0</v>
-      </c>
-      <c r="N17" s="14">
-        <v>1</v>
-      </c>
-      <c r="O17" s="14">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
+      <c r="N17" s="11">
+        <v>5</v>
+      </c>
+      <c r="O17" s="11">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>259</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>224</v>
+      <c r="B18" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>318</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="11">
         <v>0</v>
       </c>
-      <c r="N18" s="14">
-        <v>1</v>
-      </c>
-      <c r="O18" s="14">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
+      <c r="N18" s="11">
+        <v>5</v>
+      </c>
+      <c r="O18" s="11">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>224</v>
+      <c r="B19" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>318</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G19" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="14">
+        <v>2</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="11">
         <v>0</v>
       </c>
-      <c r="N19" s="14">
-        <v>1</v>
-      </c>
-      <c r="O19" s="14">
-        <v>1E-3</v>
+      <c r="N19" s="11">
+        <v>5</v>
+      </c>
+      <c r="O19" s="11">
+        <v>0.01</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>224</v>
+      <c r="B20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>318</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G20" s="14">
+        <v>2.5</v>
+      </c>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="11">
         <v>0</v>
       </c>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="14">
+      <c r="N20" s="11">
+        <v>5</v>
+      </c>
+      <c r="O20" s="11">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="14">
         <v>0</v>
       </c>
-      <c r="N20" s="14">
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="14">
+        <v>0</v>
+      </c>
+      <c r="N21" s="14">
         <v>1</v>
       </c>
-      <c r="O20" s="14">
+      <c r="O21" s="14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="14">
+        <v>0</v>
+      </c>
+      <c r="N22" s="14">
+        <v>1</v>
+      </c>
+      <c r="O22" s="14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="14">
+        <v>0</v>
+      </c>
+      <c r="N23" s="14">
+        <v>1</v>
+      </c>
+      <c r="O23" s="14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="14">
+        <v>0</v>
+      </c>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="14">
+        <v>0</v>
+      </c>
+      <c r="N24" s="14">
+        <v>1</v>
+      </c>
+      <c r="O24" s="14">
         <v>1E-3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G2:L14 G16:L20">
-    <cfRule type="expression" dxfId="319" priority="70">
+  <conditionalFormatting sqref="G2:L16 G21:L24">
+    <cfRule type="expression" dxfId="323" priority="76">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16 A2:A14 D3:D7 A16:A20">
-    <cfRule type="expression" dxfId="318" priority="48">
+  <conditionalFormatting sqref="D16 A2:A14 D3:D7 A16 A15:B15 A21:A24">
+    <cfRule type="expression" dxfId="322" priority="54">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="317" priority="49">
+    <cfRule type="expression" dxfId="321" priority="55">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:L2 B16:C16 E16 B3:C11 E3:L4 E5:E11 B12:E14 F5:L14 F16:F20 G16:L16">
-    <cfRule type="expression" dxfId="316" priority="145">
+  <conditionalFormatting sqref="B2:L2 B16:C16 B3:C11 E3:L4 E5:E11 B12:E14 F5:L14 E16:L16 F21:F24">
+    <cfRule type="expression" dxfId="320" priority="151">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="315" priority="11">
+    <cfRule type="expression" dxfId="319" priority="17">
       <formula>ISBLANK($F9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="314" priority="10">
+    <cfRule type="expression" dxfId="318" priority="16">
       <formula>ISBLANK($F10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="expression" dxfId="313" priority="9">
+    <cfRule type="expression" dxfId="317" priority="15">
       <formula>ISBLANK($F8)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="312" priority="8">
+    <cfRule type="expression" dxfId="316" priority="14">
       <formula>ISBLANK($F11)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G15:L15">
-    <cfRule type="expression" dxfId="311" priority="1">
-      <formula>NOT((COLUMN(G15)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F15, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15:B15">
-    <cfRule type="expression" dxfId="310" priority="3">
-      <formula>ISBLANK($F15)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="309" priority="4">
-      <formula>NOT((COLUMN(A15)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F15, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C15:L15">
-    <cfRule type="expression" dxfId="308" priority="2">
+    <cfRule type="expression" dxfId="315" priority="8">
       <formula>ISBLANK($F15)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H17:L20">
+    <cfRule type="expression" dxfId="314" priority="5">
+      <formula>NOT((COLUMN(H17)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F17, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17:A20 D17:D20">
+    <cfRule type="expression" dxfId="313" priority="3">
+      <formula>ISBLANK($F17)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="312" priority="4">
+      <formula>NOT((COLUMN(A17)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F17, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:C20 E17:F20 H17:L20">
+    <cfRule type="expression" dxfId="311" priority="6">
+      <formula>ISBLANK($F17)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17:G20">
+    <cfRule type="expression" dxfId="310" priority="1">
+      <formula>NOT((COLUMN(G17)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F17, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F20" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F24" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>
@@ -15076,8 +15729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87277472-6F92-4209-B3A9-C72FCC829F3A}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15408,13 +16061,13 @@
         <v>45</v>
       </c>
       <c r="C9" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="E9" s="11" t="s">
         <v>295</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>296</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>3</v>
@@ -15445,13 +16098,13 @@
         <v>45</v>
       </c>
       <c r="C10" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>298</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>299</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>3</v>
@@ -15482,13 +16135,13 @@
         <v>45</v>
       </c>
       <c r="C11" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>300</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>301</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>302</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>3</v>
@@ -15778,13 +16431,13 @@
         <v>32</v>
       </c>
       <c r="C19" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="D19" s="14" t="s">
         <v>303</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="E19" s="14" t="s">
         <v>304</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>305</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>3</v>
@@ -16114,7 +16767,7 @@
         <v>211</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>34</v>
@@ -16148,10 +16801,10 @@
         <v>32</v>
       </c>
       <c r="C29" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>307</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>308</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>187</v>
@@ -16185,10 +16838,10 @@
         <v>32</v>
       </c>
       <c r="C30" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="D30" s="11" t="s">
         <v>309</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>310</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>191</v>
@@ -16222,10 +16875,10 @@
         <v>45</v>
       </c>
       <c r="C31" s="14" t="s">
+        <v>310</v>
+      </c>
+      <c r="D31" s="14" t="s">
         <v>311</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>312</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>224</v>
@@ -16253,27 +16906,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:L31">
-    <cfRule type="expression" dxfId="290" priority="2">
+    <cfRule type="expression" dxfId="292" priority="2">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17 D12 D3:D6 D28 A2:A31">
-    <cfRule type="expression" dxfId="289" priority="3">
+    <cfRule type="expression" dxfId="291" priority="3">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:L18 B8:L11 F12:F24">
-    <cfRule type="expression" dxfId="288" priority="4">
+    <cfRule type="expression" dxfId="290" priority="4">
       <formula>ISBLANK($F8)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:L2 B18:E18 B17:C17 E17 B12:C12 E12 B3:C6 E3:L6 B13:E16 B7:L7">
-    <cfRule type="expression" dxfId="287" priority="5">
+    <cfRule type="expression" dxfId="289" priority="5">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:L30">
-    <cfRule type="expression" dxfId="286" priority="1">
+    <cfRule type="expression" dxfId="288" priority="1">
       <formula>ISBLANK($F29)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16614,20 +17267,20 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L8">
-    <cfRule type="expression" dxfId="269" priority="26">
+    <cfRule type="expression" dxfId="271" priority="26">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A8">
-    <cfRule type="expression" dxfId="268" priority="1">
+    <cfRule type="expression" dxfId="270" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="267" priority="2">
+    <cfRule type="expression" dxfId="269" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:L8">
-    <cfRule type="expression" dxfId="266" priority="129">
+    <cfRule type="expression" dxfId="268" priority="129">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Implemented sample shipping time with overnight shipping as the default
</commit_message>
<xml_diff>
--- a/Battelle.EPA.WideAreaDecon.Model.Tests/InputFiles/ModifyParametersTest.xlsx
+++ b/Battelle.EPA.WideAreaDecon.Model.Tests/InputFiles/ModifyParametersTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Documents\Tasking\(4) Wide Area Decon\Task 5 Repo\WideAreaDecon\Battelle.EPA.WideAreaDecon.Model.Tests\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C624B9C-F290-4CDF-9CD5-18FDB66BA8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84A1B15-5998-4FE9-9F1C-00CFF1BBAD5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="0" windowWidth="23016" windowHeight="12360" tabRatio="657" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="657" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1639" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1639" uniqueCount="316">
   <si>
     <t>SCWAD</t>
   </si>
@@ -690,18 +690,12 @@
     <t>unitless</t>
   </si>
   <si>
-    <t>meters</t>
-  </si>
-  <si>
     <t>hours</t>
   </si>
   <si>
     <t>Time required to transmit analysis results from external labs to Incident Command</t>
   </si>
   <si>
-    <t>Distance of each external lab from the contamination site</t>
-  </si>
-  <si>
     <t>$ / ticket</t>
   </si>
   <si>
@@ -717,9 +711,6 @@
     <t>Lab Throughput Samples per Day</t>
   </si>
   <si>
-    <t>Lab Distance from Site</t>
-  </si>
-  <si>
     <t>Hours per Entry per Team</t>
   </si>
   <si>
@@ -1006,6 +997,12 @@
   </si>
   <si>
     <t>Decon, Drying, and Venting Days</t>
+  </si>
+  <si>
+    <t>Sample Shipping Time</t>
+  </si>
+  <si>
+    <t>Amount of time it takes to ship samples to labs</t>
   </si>
 </sst>
 </file>
@@ -1327,7 +1324,43 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="422">
+  <dxfs count="426">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -7852,459 +7885,459 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table156" displayName="Table156" ref="A1:O8" totalsRowShown="0" tableBorderDxfId="416">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table156" displayName="Table156" ref="A1:O8" totalsRowShown="0" tableBorderDxfId="420">
   <autoFilter ref="A1:O8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Phase" dataDxfId="415"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category" dataDxfId="414"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="413"/>
-    <tableColumn id="10" xr3:uid="{DA69379A-DE3F-42F4-AF70-91A1718AB7E0}" name="Description" dataDxfId="412"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Units" dataDxfId="411"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Distribution Type" dataDxfId="410"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parameter 1" dataDxfId="409"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Parameter 2" dataDxfId="408"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Parameter 3" dataDxfId="407"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Parameter 4" dataDxfId="406"/>
-    <tableColumn id="14" xr3:uid="{50465694-0FC6-4F52-BBDD-C2367DABB3F3}" name="Parameter 5" dataDxfId="405"/>
-    <tableColumn id="15" xr3:uid="{9D83EAB9-CB4C-4600-AF1C-4966CB714685}" name="Parameter 6" dataDxfId="404"/>
-    <tableColumn id="11" xr3:uid="{6D5D89BA-F5B6-48D7-8EB6-F84737897B28}" name="Lower Limit" dataDxfId="403"/>
-    <tableColumn id="12" xr3:uid="{48C3D1E7-422F-49D2-B091-B1AED1C3D586}" name="Upper Limit" dataDxfId="402"/>
-    <tableColumn id="13" xr3:uid="{C7F66B6D-AE49-4F19-BA50-224FF50E099F}" name="Step" dataDxfId="401"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Phase" dataDxfId="419"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category" dataDxfId="418"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="417"/>
+    <tableColumn id="10" xr3:uid="{DA69379A-DE3F-42F4-AF70-91A1718AB7E0}" name="Description" dataDxfId="416"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Units" dataDxfId="415"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Distribution Type" dataDxfId="414"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parameter 1" dataDxfId="413"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Parameter 2" dataDxfId="412"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Parameter 3" dataDxfId="411"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Parameter 4" dataDxfId="410"/>
+    <tableColumn id="14" xr3:uid="{50465694-0FC6-4F52-BBDD-C2367DABB3F3}" name="Parameter 5" dataDxfId="409"/>
+    <tableColumn id="15" xr3:uid="{9D83EAB9-CB4C-4600-AF1C-4966CB714685}" name="Parameter 6" dataDxfId="408"/>
+    <tableColumn id="11" xr3:uid="{6D5D89BA-F5B6-48D7-8EB6-F84737897B28}" name="Lower Limit" dataDxfId="407"/>
+    <tableColumn id="12" xr3:uid="{48C3D1E7-422F-49D2-B091-B1AED1C3D586}" name="Upper Limit" dataDxfId="406"/>
+    <tableColumn id="13" xr3:uid="{C7F66B6D-AE49-4F19-BA50-224FF50E099F}" name="Step" dataDxfId="405"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3CB8E65B-B7DB-4610-98F8-15D74050538C}" name="Table156410" displayName="Table156410" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="199" tableBorderDxfId="198">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3CB8E65B-B7DB-4610-98F8-15D74050538C}" name="Table156410" displayName="Table156410" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="203" tableBorderDxfId="202">
   <autoFilter ref="A1:O2" xr:uid="{A2DF75BF-F49D-463D-B10C-635E799069A4}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{33E848DD-559D-4023-9F06-526E6AF9BD94}" name="Phase" dataDxfId="197"/>
-    <tableColumn id="20" xr3:uid="{9EDFC6C3-E3F9-4924-BC6A-804D2BBDAE4E}" name="Category" dataDxfId="196"/>
-    <tableColumn id="12" xr3:uid="{D5F0DA51-2BBD-46FF-88FA-75AA7A464F56}" name="Name" dataDxfId="195"/>
-    <tableColumn id="14" xr3:uid="{C6DADE20-FD43-4249-ADF7-72D9BB6ED860}" name="Description" dataDxfId="194"/>
-    <tableColumn id="18" xr3:uid="{017077E2-A519-4357-81FC-29BBCF542A5D}" name="Units" dataDxfId="193"/>
-    <tableColumn id="4" xr3:uid="{18A3B7BD-46E6-497D-932B-A279201CED36}" name="Distribution Type" dataDxfId="192"/>
-    <tableColumn id="5" xr3:uid="{5BD00F12-3393-4245-9BE0-D37573FCF5E3}" name="Parameter 1" dataDxfId="191"/>
-    <tableColumn id="6" xr3:uid="{F68E7FA0-23DA-4C5B-BCD3-BD3C7B299B02}" name="Parameter 2" dataDxfId="190"/>
-    <tableColumn id="7" xr3:uid="{E074689D-E9A9-4D78-901F-4D6DEAB8F157}" name="Parameter 3" dataDxfId="189"/>
-    <tableColumn id="10" xr3:uid="{24FDA3C5-E39C-430C-90BB-3F6BD09EEDC7}" name="Parameter 4" dataDxfId="188"/>
-    <tableColumn id="11" xr3:uid="{42BED06C-CBA3-4453-AE89-CFE7799A8559}" name="Parameter 5" dataDxfId="187"/>
-    <tableColumn id="8" xr3:uid="{4CFE8BFF-6747-408C-8ABA-AFDB589C4F81}" name="Parameter 6" dataDxfId="186"/>
-    <tableColumn id="15" xr3:uid="{E0BBD4D8-EA8D-4CAF-B849-F7A2CE769A48}" name="Lower Limit" dataDxfId="185"/>
-    <tableColumn id="16" xr3:uid="{4800A8E8-843B-4C41-91BF-C1A3C30DE8D6}" name="Upper Limit" dataDxfId="184"/>
-    <tableColumn id="17" xr3:uid="{A6367C3F-1F51-48D6-9EB3-E8501CEA0DC3}" name="Step" dataDxfId="183"/>
+    <tableColumn id="9" xr3:uid="{33E848DD-559D-4023-9F06-526E6AF9BD94}" name="Phase" dataDxfId="201"/>
+    <tableColumn id="20" xr3:uid="{9EDFC6C3-E3F9-4924-BC6A-804D2BBDAE4E}" name="Category" dataDxfId="200"/>
+    <tableColumn id="12" xr3:uid="{D5F0DA51-2BBD-46FF-88FA-75AA7A464F56}" name="Name" dataDxfId="199"/>
+    <tableColumn id="14" xr3:uid="{C6DADE20-FD43-4249-ADF7-72D9BB6ED860}" name="Description" dataDxfId="198"/>
+    <tableColumn id="18" xr3:uid="{017077E2-A519-4357-81FC-29BBCF542A5D}" name="Units" dataDxfId="197"/>
+    <tableColumn id="4" xr3:uid="{18A3B7BD-46E6-497D-932B-A279201CED36}" name="Distribution Type" dataDxfId="196"/>
+    <tableColumn id="5" xr3:uid="{5BD00F12-3393-4245-9BE0-D37573FCF5E3}" name="Parameter 1" dataDxfId="195"/>
+    <tableColumn id="6" xr3:uid="{F68E7FA0-23DA-4C5B-BCD3-BD3C7B299B02}" name="Parameter 2" dataDxfId="194"/>
+    <tableColumn id="7" xr3:uid="{E074689D-E9A9-4D78-901F-4D6DEAB8F157}" name="Parameter 3" dataDxfId="193"/>
+    <tableColumn id="10" xr3:uid="{24FDA3C5-E39C-430C-90BB-3F6BD09EEDC7}" name="Parameter 4" dataDxfId="192"/>
+    <tableColumn id="11" xr3:uid="{42BED06C-CBA3-4453-AE89-CFE7799A8559}" name="Parameter 5" dataDxfId="191"/>
+    <tableColumn id="8" xr3:uid="{4CFE8BFF-6747-408C-8ABA-AFDB589C4F81}" name="Parameter 6" dataDxfId="190"/>
+    <tableColumn id="15" xr3:uid="{E0BBD4D8-EA8D-4CAF-B849-F7A2CE769A48}" name="Lower Limit" dataDxfId="189"/>
+    <tableColumn id="16" xr3:uid="{4800A8E8-843B-4C41-91BF-C1A3C30DE8D6}" name="Upper Limit" dataDxfId="188"/>
+    <tableColumn id="17" xr3:uid="{A6367C3F-1F51-48D6-9EB3-E8501CEA0DC3}" name="Step" dataDxfId="187"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{86A1116E-A4B1-4819-B8BD-755AC0F1A27A}" name="Table15648" displayName="Table15648" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="178" tableBorderDxfId="177">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{86A1116E-A4B1-4819-B8BD-755AC0F1A27A}" name="Table15648" displayName="Table15648" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="182" tableBorderDxfId="181">
   <autoFilter ref="A1:O2" xr:uid="{990E6A50-401C-443A-9431-A3C6B1C33DB9}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{B7EF7E94-8BD1-4B05-A1E1-DE0166BDA299}" name="Phase" dataDxfId="176"/>
-    <tableColumn id="20" xr3:uid="{3E394D25-22F5-47DE-8DD2-1B412C8ACB40}" name="Category" dataDxfId="175"/>
-    <tableColumn id="12" xr3:uid="{581C35A5-6B54-4CCA-AD27-A0086A458CD9}" name="Name" dataDxfId="174"/>
-    <tableColumn id="14" xr3:uid="{02601854-7EF0-4B53-83BA-E1A583AB0E89}" name="Description" dataDxfId="173"/>
-    <tableColumn id="18" xr3:uid="{38E6F539-D589-4AEB-9FF3-0F3407B1F600}" name="Units" dataDxfId="172"/>
-    <tableColumn id="4" xr3:uid="{758D0224-FF70-4B51-A43F-A666DBEE60B5}" name="Distribution Type" dataDxfId="171"/>
-    <tableColumn id="5" xr3:uid="{AA403007-B0D8-4F37-BBED-A39F4CBEC713}" name="Parameter 1" dataDxfId="170"/>
-    <tableColumn id="6" xr3:uid="{AEFD9020-CB8D-46C6-A545-72935F5E17C9}" name="Parameter 2" dataDxfId="169"/>
-    <tableColumn id="7" xr3:uid="{5391F637-3141-4924-AB2D-BB7560C402FC}" name="Parameter 3" dataDxfId="168"/>
-    <tableColumn id="10" xr3:uid="{DD30C7A0-FB24-4548-956F-070EED2E392A}" name="Parameter 4" dataDxfId="167"/>
-    <tableColumn id="11" xr3:uid="{4C51B414-DF9A-46F4-A761-171654CD826B}" name="Parameter 5" dataDxfId="166"/>
-    <tableColumn id="8" xr3:uid="{C36C5078-BCC8-4902-86B0-4CC5F5B94354}" name="Parameter 6" dataDxfId="165"/>
-    <tableColumn id="15" xr3:uid="{0B417314-7BF7-498C-AFAD-AF435E3794CB}" name="Lower Limit" dataDxfId="164"/>
-    <tableColumn id="16" xr3:uid="{869CD7E5-A5F2-42BE-860A-4654BBA29091}" name="Upper Limit" dataDxfId="163"/>
-    <tableColumn id="17" xr3:uid="{9D5645C4-35FE-4467-8F7A-0259A9E00D72}" name="Step" dataDxfId="162"/>
+    <tableColumn id="9" xr3:uid="{B7EF7E94-8BD1-4B05-A1E1-DE0166BDA299}" name="Phase" dataDxfId="180"/>
+    <tableColumn id="20" xr3:uid="{3E394D25-22F5-47DE-8DD2-1B412C8ACB40}" name="Category" dataDxfId="179"/>
+    <tableColumn id="12" xr3:uid="{581C35A5-6B54-4CCA-AD27-A0086A458CD9}" name="Name" dataDxfId="178"/>
+    <tableColumn id="14" xr3:uid="{02601854-7EF0-4B53-83BA-E1A583AB0E89}" name="Description" dataDxfId="177"/>
+    <tableColumn id="18" xr3:uid="{38E6F539-D589-4AEB-9FF3-0F3407B1F600}" name="Units" dataDxfId="176"/>
+    <tableColumn id="4" xr3:uid="{758D0224-FF70-4B51-A43F-A666DBEE60B5}" name="Distribution Type" dataDxfId="175"/>
+    <tableColumn id="5" xr3:uid="{AA403007-B0D8-4F37-BBED-A39F4CBEC713}" name="Parameter 1" dataDxfId="174"/>
+    <tableColumn id="6" xr3:uid="{AEFD9020-CB8D-46C6-A545-72935F5E17C9}" name="Parameter 2" dataDxfId="173"/>
+    <tableColumn id="7" xr3:uid="{5391F637-3141-4924-AB2D-BB7560C402FC}" name="Parameter 3" dataDxfId="172"/>
+    <tableColumn id="10" xr3:uid="{DD30C7A0-FB24-4548-956F-070EED2E392A}" name="Parameter 4" dataDxfId="171"/>
+    <tableColumn id="11" xr3:uid="{4C51B414-DF9A-46F4-A761-171654CD826B}" name="Parameter 5" dataDxfId="170"/>
+    <tableColumn id="8" xr3:uid="{C36C5078-BCC8-4902-86B0-4CC5F5B94354}" name="Parameter 6" dataDxfId="169"/>
+    <tableColumn id="15" xr3:uid="{0B417314-7BF7-498C-AFAD-AF435E3794CB}" name="Lower Limit" dataDxfId="168"/>
+    <tableColumn id="16" xr3:uid="{869CD7E5-A5F2-42BE-860A-4654BBA29091}" name="Upper Limit" dataDxfId="167"/>
+    <tableColumn id="17" xr3:uid="{9D5645C4-35FE-4467-8F7A-0259A9E00D72}" name="Step" dataDxfId="166"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{70557EE6-CCDF-497F-AD58-5C0E1C74D197}" name="Table156412" displayName="Table156412" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="157" tableBorderDxfId="156">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{70557EE6-CCDF-497F-AD58-5C0E1C74D197}" name="Table156412" displayName="Table156412" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="161" tableBorderDxfId="160">
   <autoFilter ref="A1:O2" xr:uid="{98B9CAE8-5809-471F-A0E6-3C63C0FF7931}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{0E927F65-2069-4507-B0B0-8DA725AF99EC}" name="Phase" dataDxfId="155"/>
-    <tableColumn id="20" xr3:uid="{921518C6-F6AF-4306-9A67-62C12E697D60}" name="Category" dataDxfId="154"/>
-    <tableColumn id="12" xr3:uid="{CD5679ED-CB25-488E-8C70-2C446DAB28DC}" name="Name" dataDxfId="153"/>
-    <tableColumn id="14" xr3:uid="{F17E92B1-609F-453F-8FC2-11AB75FFB5B0}" name="Description" dataDxfId="152"/>
-    <tableColumn id="18" xr3:uid="{CA25841B-E30A-4228-B65F-216207437CB0}" name="Units" dataDxfId="151"/>
-    <tableColumn id="4" xr3:uid="{5CF3C293-70A2-445C-B6F4-D4BCEB868AEC}" name="Distribution Type" dataDxfId="150"/>
-    <tableColumn id="5" xr3:uid="{6B896B7D-F74D-42FF-97BC-93D69E611504}" name="Parameter 1" dataDxfId="149"/>
-    <tableColumn id="6" xr3:uid="{02AE94F0-B427-476D-88EB-3C9235866F4E}" name="Parameter 2" dataDxfId="148"/>
-    <tableColumn id="7" xr3:uid="{C0EF4425-A63A-42D7-82B9-4C1366C7BF01}" name="Parameter 3" dataDxfId="147"/>
-    <tableColumn id="10" xr3:uid="{7F665756-5949-4CD6-AE8C-F7531D7A9CAD}" name="Parameter 4" dataDxfId="146"/>
-    <tableColumn id="11" xr3:uid="{59049478-1CD8-416F-BED1-BD7B8FEA0C41}" name="Parameter 5" dataDxfId="145"/>
-    <tableColumn id="8" xr3:uid="{CC7DFE3F-C2E2-4F46-B153-D03CF263B523}" name="Parameter 6" dataDxfId="144"/>
-    <tableColumn id="15" xr3:uid="{F2A6353F-D73A-41E5-B265-D8F18AA4409C}" name="Lower Limit" dataDxfId="143"/>
-    <tableColumn id="16" xr3:uid="{1D8D56B8-5F2C-48C5-9CE4-93C38BD7488F}" name="Upper Limit" dataDxfId="142"/>
-    <tableColumn id="17" xr3:uid="{6AB8DBB9-751A-4840-BC73-4780E1B009AD}" name="Step" dataDxfId="141"/>
+    <tableColumn id="9" xr3:uid="{0E927F65-2069-4507-B0B0-8DA725AF99EC}" name="Phase" dataDxfId="159"/>
+    <tableColumn id="20" xr3:uid="{921518C6-F6AF-4306-9A67-62C12E697D60}" name="Category" dataDxfId="158"/>
+    <tableColumn id="12" xr3:uid="{CD5679ED-CB25-488E-8C70-2C446DAB28DC}" name="Name" dataDxfId="157"/>
+    <tableColumn id="14" xr3:uid="{F17E92B1-609F-453F-8FC2-11AB75FFB5B0}" name="Description" dataDxfId="156"/>
+    <tableColumn id="18" xr3:uid="{CA25841B-E30A-4228-B65F-216207437CB0}" name="Units" dataDxfId="155"/>
+    <tableColumn id="4" xr3:uid="{5CF3C293-70A2-445C-B6F4-D4BCEB868AEC}" name="Distribution Type" dataDxfId="154"/>
+    <tableColumn id="5" xr3:uid="{6B896B7D-F74D-42FF-97BC-93D69E611504}" name="Parameter 1" dataDxfId="153"/>
+    <tableColumn id="6" xr3:uid="{02AE94F0-B427-476D-88EB-3C9235866F4E}" name="Parameter 2" dataDxfId="152"/>
+    <tableColumn id="7" xr3:uid="{C0EF4425-A63A-42D7-82B9-4C1366C7BF01}" name="Parameter 3" dataDxfId="151"/>
+    <tableColumn id="10" xr3:uid="{7F665756-5949-4CD6-AE8C-F7531D7A9CAD}" name="Parameter 4" dataDxfId="150"/>
+    <tableColumn id="11" xr3:uid="{59049478-1CD8-416F-BED1-BD7B8FEA0C41}" name="Parameter 5" dataDxfId="149"/>
+    <tableColumn id="8" xr3:uid="{CC7DFE3F-C2E2-4F46-B153-D03CF263B523}" name="Parameter 6" dataDxfId="148"/>
+    <tableColumn id="15" xr3:uid="{F2A6353F-D73A-41E5-B265-D8F18AA4409C}" name="Lower Limit" dataDxfId="147"/>
+    <tableColumn id="16" xr3:uid="{1D8D56B8-5F2C-48C5-9CE4-93C38BD7488F}" name="Upper Limit" dataDxfId="146"/>
+    <tableColumn id="17" xr3:uid="{6AB8DBB9-751A-4840-BC73-4780E1B009AD}" name="Step" dataDxfId="145"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{F9C17F91-E3F1-4ABE-9219-5A5F8F4C3152}" name="Table1564518" displayName="Table1564518" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="136" tableBorderDxfId="135">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{F9C17F91-E3F1-4ABE-9219-5A5F8F4C3152}" name="Table1564518" displayName="Table1564518" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="140" tableBorderDxfId="139">
   <autoFilter ref="A1:O2" xr:uid="{CE70FAE3-DAD6-40A6-BCCE-F46A2CDA0980}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{77AC217A-782C-47D2-9945-D4226DB02CB4}" name="Phase" dataDxfId="134"/>
-    <tableColumn id="22" xr3:uid="{A77A81F7-C018-4F6E-BF69-5FE486BECF62}" name="Category" dataDxfId="133"/>
-    <tableColumn id="12" xr3:uid="{CCA10716-C2B0-4055-953E-1957EC05B7DC}" name="Name" dataDxfId="132"/>
-    <tableColumn id="14" xr3:uid="{9131E52D-9D7C-41BF-ABF5-9AAF65D5BC39}" name="Description" dataDxfId="131"/>
-    <tableColumn id="18" xr3:uid="{819C7026-BBE6-4FEF-81FC-063CF9E923E1}" name="Units" dataDxfId="130"/>
-    <tableColumn id="4" xr3:uid="{BCC0BC54-494B-4CD2-9D93-4A14A321EFDE}" name="Distribution Type" dataDxfId="129"/>
-    <tableColumn id="5" xr3:uid="{890B6437-FEB3-4225-BE1D-8F4BB30A2A95}" name="Parameter 1" dataDxfId="128"/>
-    <tableColumn id="6" xr3:uid="{D95452BF-5FFC-4C2D-BE8B-1138CADE3867}" name="Parameter 2" dataDxfId="127"/>
-    <tableColumn id="7" xr3:uid="{AFAD290F-88ED-4F65-8343-1B7E0B2331C2}" name="Parameter 3" dataDxfId="126"/>
-    <tableColumn id="10" xr3:uid="{C7581E5C-58E6-4080-A3F0-3C90449EE32D}" name="Parameter 4" dataDxfId="125"/>
-    <tableColumn id="11" xr3:uid="{1D5C967F-8BEE-4049-9B30-056174F945AE}" name="Parameter 5" dataDxfId="124"/>
-    <tableColumn id="8" xr3:uid="{058E5821-3943-44C1-B08D-F22618A8CB01}" name="Parameter 6" dataDxfId="123"/>
-    <tableColumn id="15" xr3:uid="{C95BAD13-0F40-4073-97D7-EA904AFBC77C}" name="Lower Limit" dataDxfId="122"/>
-    <tableColumn id="16" xr3:uid="{582C9B39-6E23-469E-818C-CDD30AA83C2C}" name="Upper Limit" dataDxfId="121"/>
-    <tableColumn id="17" xr3:uid="{27D6A1B7-E56F-410E-929C-C8BD6000D2D9}" name="Step" dataDxfId="120"/>
+    <tableColumn id="9" xr3:uid="{77AC217A-782C-47D2-9945-D4226DB02CB4}" name="Phase" dataDxfId="138"/>
+    <tableColumn id="22" xr3:uid="{A77A81F7-C018-4F6E-BF69-5FE486BECF62}" name="Category" dataDxfId="137"/>
+    <tableColumn id="12" xr3:uid="{CCA10716-C2B0-4055-953E-1957EC05B7DC}" name="Name" dataDxfId="136"/>
+    <tableColumn id="14" xr3:uid="{9131E52D-9D7C-41BF-ABF5-9AAF65D5BC39}" name="Description" dataDxfId="135"/>
+    <tableColumn id="18" xr3:uid="{819C7026-BBE6-4FEF-81FC-063CF9E923E1}" name="Units" dataDxfId="134"/>
+    <tableColumn id="4" xr3:uid="{BCC0BC54-494B-4CD2-9D93-4A14A321EFDE}" name="Distribution Type" dataDxfId="133"/>
+    <tableColumn id="5" xr3:uid="{890B6437-FEB3-4225-BE1D-8F4BB30A2A95}" name="Parameter 1" dataDxfId="132"/>
+    <tableColumn id="6" xr3:uid="{D95452BF-5FFC-4C2D-BE8B-1138CADE3867}" name="Parameter 2" dataDxfId="131"/>
+    <tableColumn id="7" xr3:uid="{AFAD290F-88ED-4F65-8343-1B7E0B2331C2}" name="Parameter 3" dataDxfId="130"/>
+    <tableColumn id="10" xr3:uid="{C7581E5C-58E6-4080-A3F0-3C90449EE32D}" name="Parameter 4" dataDxfId="129"/>
+    <tableColumn id="11" xr3:uid="{1D5C967F-8BEE-4049-9B30-056174F945AE}" name="Parameter 5" dataDxfId="128"/>
+    <tableColumn id="8" xr3:uid="{058E5821-3943-44C1-B08D-F22618A8CB01}" name="Parameter 6" dataDxfId="127"/>
+    <tableColumn id="15" xr3:uid="{C95BAD13-0F40-4073-97D7-EA904AFBC77C}" name="Lower Limit" dataDxfId="126"/>
+    <tableColumn id="16" xr3:uid="{582C9B39-6E23-469E-818C-CDD30AA83C2C}" name="Upper Limit" dataDxfId="125"/>
+    <tableColumn id="17" xr3:uid="{27D6A1B7-E56F-410E-929C-C8BD6000D2D9}" name="Step" dataDxfId="124"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{432F1329-A516-4974-97D5-CED039B9825E}" name="Table15649" displayName="Table15649" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="115" tableBorderDxfId="114">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{432F1329-A516-4974-97D5-CED039B9825E}" name="Table15649" displayName="Table15649" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="119" tableBorderDxfId="118">
   <autoFilter ref="A1:O2" xr:uid="{68B29069-2622-4242-A0DD-EA343A9BF637}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{A65D510F-11AE-4758-A918-595CFAEACDBA}" name="Phase" dataDxfId="113"/>
-    <tableColumn id="20" xr3:uid="{1983ED84-E3C7-438C-9FBC-6F68009993BF}" name="Category" dataDxfId="112"/>
-    <tableColumn id="12" xr3:uid="{5F8CF16A-5A1F-471D-941E-E8FA15DC40D9}" name="Name" dataDxfId="111"/>
-    <tableColumn id="14" xr3:uid="{603CB562-B188-4D78-8AF7-0C257FE01A78}" name="Description" dataDxfId="110"/>
-    <tableColumn id="18" xr3:uid="{25C96984-595F-4E53-AEA3-48FE8964668C}" name="Units" dataDxfId="109"/>
-    <tableColumn id="4" xr3:uid="{3AC7C66C-7352-42C7-A88A-718F1163EBC3}" name="Distribution Type" dataDxfId="108"/>
-    <tableColumn id="5" xr3:uid="{6CD1BB89-2672-4A45-AE6D-45DC8FD8C2D0}" name="Parameter 1" dataDxfId="107"/>
-    <tableColumn id="6" xr3:uid="{713F99C9-7865-434B-9380-0F8833A0B7CE}" name="Parameter 2" dataDxfId="106"/>
-    <tableColumn id="7" xr3:uid="{7B3CBF6D-ABAD-435C-93E5-94B2A9A1570D}" name="Parameter 3" dataDxfId="105"/>
-    <tableColumn id="10" xr3:uid="{FD8F6808-F8E5-4346-BE6E-D40A5DADECAC}" name="Parameter 4" dataDxfId="104"/>
-    <tableColumn id="11" xr3:uid="{DC3102D4-541E-44FE-AEFA-0FB92AC933C5}" name="Parameter 5" dataDxfId="103"/>
-    <tableColumn id="8" xr3:uid="{151C5968-B156-4013-B6C4-5D012F22EEF6}" name="Parameter 6" dataDxfId="102"/>
-    <tableColumn id="15" xr3:uid="{868EF292-2E08-40B9-9605-DAF748095734}" name="Lower Limit" dataDxfId="101"/>
-    <tableColumn id="16" xr3:uid="{42D5D159-9DC2-4FE5-9923-4E2B98164CE9}" name="Upper Limit" dataDxfId="100"/>
-    <tableColumn id="17" xr3:uid="{10AFF230-51CB-4644-8521-A18EFFD37E36}" name="Step" dataDxfId="99"/>
+    <tableColumn id="9" xr3:uid="{A65D510F-11AE-4758-A918-595CFAEACDBA}" name="Phase" dataDxfId="117"/>
+    <tableColumn id="20" xr3:uid="{1983ED84-E3C7-438C-9FBC-6F68009993BF}" name="Category" dataDxfId="116"/>
+    <tableColumn id="12" xr3:uid="{5F8CF16A-5A1F-471D-941E-E8FA15DC40D9}" name="Name" dataDxfId="115"/>
+    <tableColumn id="14" xr3:uid="{603CB562-B188-4D78-8AF7-0C257FE01A78}" name="Description" dataDxfId="114"/>
+    <tableColumn id="18" xr3:uid="{25C96984-595F-4E53-AEA3-48FE8964668C}" name="Units" dataDxfId="113"/>
+    <tableColumn id="4" xr3:uid="{3AC7C66C-7352-42C7-A88A-718F1163EBC3}" name="Distribution Type" dataDxfId="112"/>
+    <tableColumn id="5" xr3:uid="{6CD1BB89-2672-4A45-AE6D-45DC8FD8C2D0}" name="Parameter 1" dataDxfId="111"/>
+    <tableColumn id="6" xr3:uid="{713F99C9-7865-434B-9380-0F8833A0B7CE}" name="Parameter 2" dataDxfId="110"/>
+    <tableColumn id="7" xr3:uid="{7B3CBF6D-ABAD-435C-93E5-94B2A9A1570D}" name="Parameter 3" dataDxfId="109"/>
+    <tableColumn id="10" xr3:uid="{FD8F6808-F8E5-4346-BE6E-D40A5DADECAC}" name="Parameter 4" dataDxfId="108"/>
+    <tableColumn id="11" xr3:uid="{DC3102D4-541E-44FE-AEFA-0FB92AC933C5}" name="Parameter 5" dataDxfId="107"/>
+    <tableColumn id="8" xr3:uid="{151C5968-B156-4013-B6C4-5D012F22EEF6}" name="Parameter 6" dataDxfId="106"/>
+    <tableColumn id="15" xr3:uid="{868EF292-2E08-40B9-9605-DAF748095734}" name="Lower Limit" dataDxfId="105"/>
+    <tableColumn id="16" xr3:uid="{42D5D159-9DC2-4FE5-9923-4E2B98164CE9}" name="Upper Limit" dataDxfId="104"/>
+    <tableColumn id="17" xr3:uid="{10AFF230-51CB-4644-8521-A18EFFD37E36}" name="Step" dataDxfId="103"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{DF020213-F975-452A-9830-6EF38DDE7DCF}" name="Table15647" displayName="Table15647" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="96" tableBorderDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{DF020213-F975-452A-9830-6EF38DDE7DCF}" name="Table15647" displayName="Table15647" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="100" tableBorderDxfId="99">
   <autoFilter ref="A1:O2" xr:uid="{859BD2B0-AA02-48BA-8620-BDF827813892}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{F237A42D-415A-475B-91B7-8CB0D38B7028}" name="Phase" dataDxfId="94"/>
-    <tableColumn id="20" xr3:uid="{D2304797-990E-4466-8277-ACC378FC5EF1}" name="Category" dataDxfId="93"/>
-    <tableColumn id="12" xr3:uid="{E8D03348-3348-4698-9DA9-FDFD93C4108D}" name="Name" dataDxfId="92"/>
-    <tableColumn id="14" xr3:uid="{D9BE976B-814C-40BA-BB9C-F5A4A863809D}" name="Description" dataDxfId="91"/>
-    <tableColumn id="18" xr3:uid="{C8EEDF00-53C4-4BBB-A736-4C222CC37ACE}" name="Units" dataDxfId="90"/>
-    <tableColumn id="4" xr3:uid="{B912A136-218A-46A6-9298-A26FF451BC8B}" name="Distribution Type" dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{B469F8C6-AC37-4E2C-B435-D79806B5EB80}" name="Parameter 1" dataDxfId="88"/>
-    <tableColumn id="6" xr3:uid="{6E4BE98D-3625-46DA-8047-5C4657A18F62}" name="Parameter 2" dataDxfId="87"/>
-    <tableColumn id="7" xr3:uid="{24844D85-F2B8-4B62-9347-EE51DBA7335D}" name="Parameter 3" dataDxfId="86"/>
-    <tableColumn id="10" xr3:uid="{A09FB262-3AAD-46E1-B780-FAC155246DCB}" name="Parameter 4" dataDxfId="85"/>
-    <tableColumn id="11" xr3:uid="{C49055A9-0CD5-4B9A-9D72-65429F3A5716}" name="Parameter 5" dataDxfId="84"/>
-    <tableColumn id="8" xr3:uid="{B80ED53B-AC7B-4D83-B11D-F4584FC387E7}" name="Parameter 6" dataDxfId="83"/>
-    <tableColumn id="15" xr3:uid="{196E4D59-E5D8-47FC-8FBC-0DF83057658E}" name="Lower Limit" dataDxfId="82"/>
-    <tableColumn id="16" xr3:uid="{9EDBB862-8D13-4999-A6D8-0549867DD0D7}" name="Upper Limit" dataDxfId="81"/>
-    <tableColumn id="17" xr3:uid="{9F81C7E5-43F7-4126-A586-BB1219F70A02}" name="Step" dataDxfId="80"/>
+    <tableColumn id="9" xr3:uid="{F237A42D-415A-475B-91B7-8CB0D38B7028}" name="Phase" dataDxfId="98"/>
+    <tableColumn id="20" xr3:uid="{D2304797-990E-4466-8277-ACC378FC5EF1}" name="Category" dataDxfId="97"/>
+    <tableColumn id="12" xr3:uid="{E8D03348-3348-4698-9DA9-FDFD93C4108D}" name="Name" dataDxfId="96"/>
+    <tableColumn id="14" xr3:uid="{D9BE976B-814C-40BA-BB9C-F5A4A863809D}" name="Description" dataDxfId="95"/>
+    <tableColumn id="18" xr3:uid="{C8EEDF00-53C4-4BBB-A736-4C222CC37ACE}" name="Units" dataDxfId="94"/>
+    <tableColumn id="4" xr3:uid="{B912A136-218A-46A6-9298-A26FF451BC8B}" name="Distribution Type" dataDxfId="93"/>
+    <tableColumn id="5" xr3:uid="{B469F8C6-AC37-4E2C-B435-D79806B5EB80}" name="Parameter 1" dataDxfId="92"/>
+    <tableColumn id="6" xr3:uid="{6E4BE98D-3625-46DA-8047-5C4657A18F62}" name="Parameter 2" dataDxfId="91"/>
+    <tableColumn id="7" xr3:uid="{24844D85-F2B8-4B62-9347-EE51DBA7335D}" name="Parameter 3" dataDxfId="90"/>
+    <tableColumn id="10" xr3:uid="{A09FB262-3AAD-46E1-B780-FAC155246DCB}" name="Parameter 4" dataDxfId="89"/>
+    <tableColumn id="11" xr3:uid="{C49055A9-0CD5-4B9A-9D72-65429F3A5716}" name="Parameter 5" dataDxfId="88"/>
+    <tableColumn id="8" xr3:uid="{B80ED53B-AC7B-4D83-B11D-F4584FC387E7}" name="Parameter 6" dataDxfId="87"/>
+    <tableColumn id="15" xr3:uid="{196E4D59-E5D8-47FC-8FBC-0DF83057658E}" name="Lower Limit" dataDxfId="86"/>
+    <tableColumn id="16" xr3:uid="{9EDBB862-8D13-4999-A6D8-0549867DD0D7}" name="Upper Limit" dataDxfId="85"/>
+    <tableColumn id="17" xr3:uid="{9F81C7E5-43F7-4126-A586-BB1219F70A02}" name="Step" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{7550EFF0-9439-4E6A-8D23-02F504FBD1D4}" name="Table156414" displayName="Table156414" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="77" tableBorderDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{7550EFF0-9439-4E6A-8D23-02F504FBD1D4}" name="Table156414" displayName="Table156414" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="81" tableBorderDxfId="80">
   <autoFilter ref="A1:O2" xr:uid="{E89F1AAB-0467-4C13-8286-F7AC331E8CED}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{AE476C5A-DA1D-465E-9CDD-F6537F49B59A}" name="Phase" dataDxfId="75"/>
-    <tableColumn id="12" xr3:uid="{5D89776A-B117-4D83-ACC3-F00ADD3FE56E}" name="Category" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{9037C44A-A90D-462C-A2F2-1224467C2BC0}" name="Name" dataDxfId="73"/>
-    <tableColumn id="14" xr3:uid="{E343E4A4-9362-4305-9A92-A8062E97127D}" name="Description" dataDxfId="72"/>
-    <tableColumn id="18" xr3:uid="{59A60541-5F4F-478A-996C-A136B098D92B}" name="Units" dataDxfId="71"/>
-    <tableColumn id="4" xr3:uid="{30DA923F-FB86-4AC4-B259-AE796033AAED}" name="Distribution Type" dataDxfId="70"/>
-    <tableColumn id="5" xr3:uid="{BD9D6BB8-0A9E-48E1-95D5-0EECCBFE8316}" name="Parameter 1" dataDxfId="69"/>
-    <tableColumn id="6" xr3:uid="{B0E10190-9195-4B9D-A20D-A270CE2F3E98}" name="Parameter 2" dataDxfId="68"/>
-    <tableColumn id="7" xr3:uid="{918B726D-0E60-49F6-94FE-F7B5CF284EB2}" name="Parameter 3" dataDxfId="67"/>
-    <tableColumn id="10" xr3:uid="{F52C94ED-5667-4B4C-AF10-29D9CF45ACB5}" name="Parameter 4" dataDxfId="66"/>
-    <tableColumn id="11" xr3:uid="{9F8440AB-4D90-4F35-8265-07E520410CC0}" name="Parameter 5" dataDxfId="65"/>
-    <tableColumn id="8" xr3:uid="{4F13BDAF-F86A-4434-B9C3-576D1A4571C8}" name="Parameter 6" dataDxfId="64"/>
-    <tableColumn id="15" xr3:uid="{168B9EEC-D86A-4C57-8174-66D02451AA11}" name="Lower Limit" dataDxfId="63"/>
-    <tableColumn id="16" xr3:uid="{B91AA0FC-6FD4-4503-8497-8E2658CD5A9C}" name="Upper Limit" dataDxfId="62"/>
-    <tableColumn id="17" xr3:uid="{85F85B4E-2654-4B9F-8CBF-9AF7D4017806}" name="Step" dataDxfId="61"/>
+    <tableColumn id="9" xr3:uid="{AE476C5A-DA1D-465E-9CDD-F6537F49B59A}" name="Phase" dataDxfId="79"/>
+    <tableColumn id="12" xr3:uid="{5D89776A-B117-4D83-ACC3-F00ADD3FE56E}" name="Category" dataDxfId="78"/>
+    <tableColumn id="3" xr3:uid="{9037C44A-A90D-462C-A2F2-1224467C2BC0}" name="Name" dataDxfId="77"/>
+    <tableColumn id="14" xr3:uid="{E343E4A4-9362-4305-9A92-A8062E97127D}" name="Description" dataDxfId="76"/>
+    <tableColumn id="18" xr3:uid="{59A60541-5F4F-478A-996C-A136B098D92B}" name="Units" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{30DA923F-FB86-4AC4-B259-AE796033AAED}" name="Distribution Type" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{BD9D6BB8-0A9E-48E1-95D5-0EECCBFE8316}" name="Parameter 1" dataDxfId="73"/>
+    <tableColumn id="6" xr3:uid="{B0E10190-9195-4B9D-A20D-A270CE2F3E98}" name="Parameter 2" dataDxfId="72"/>
+    <tableColumn id="7" xr3:uid="{918B726D-0E60-49F6-94FE-F7B5CF284EB2}" name="Parameter 3" dataDxfId="71"/>
+    <tableColumn id="10" xr3:uid="{F52C94ED-5667-4B4C-AF10-29D9CF45ACB5}" name="Parameter 4" dataDxfId="70"/>
+    <tableColumn id="11" xr3:uid="{9F8440AB-4D90-4F35-8265-07E520410CC0}" name="Parameter 5" dataDxfId="69"/>
+    <tableColumn id="8" xr3:uid="{4F13BDAF-F86A-4434-B9C3-576D1A4571C8}" name="Parameter 6" dataDxfId="68"/>
+    <tableColumn id="15" xr3:uid="{168B9EEC-D86A-4C57-8174-66D02451AA11}" name="Lower Limit" dataDxfId="67"/>
+    <tableColumn id="16" xr3:uid="{B91AA0FC-6FD4-4503-8497-8E2658CD5A9C}" name="Upper Limit" dataDxfId="66"/>
+    <tableColumn id="17" xr3:uid="{85F85B4E-2654-4B9F-8CBF-9AF7D4017806}" name="Step" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{544BD654-9B18-4F85-8680-0367091A97FD}" name="Table15646" displayName="Table15646" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="56" tableBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{544BD654-9B18-4F85-8680-0367091A97FD}" name="Table15646" displayName="Table15646" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="60" tableBorderDxfId="59">
   <autoFilter ref="A1:O2" xr:uid="{EC61BB93-4EB0-4480-9F8B-C9A2D56564B4}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{1735A646-077D-4A5C-8ABA-5E5552C83F8B}" name="Phase" dataDxfId="54"/>
-    <tableColumn id="20" xr3:uid="{004108F0-B585-4FC4-8E02-24F2EDB488C0}" name="Category" dataDxfId="53"/>
-    <tableColumn id="12" xr3:uid="{69E4893D-8A0F-46ED-8648-226BDC719B2B}" name="Name" dataDxfId="52"/>
-    <tableColumn id="14" xr3:uid="{A839FAC0-08F6-4AA7-96B8-39B9A47A057D}" name="Description" dataDxfId="51"/>
-    <tableColumn id="18" xr3:uid="{E0746BE3-6AD9-4082-A683-C57740CF7686}" name="Units" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{C6BD6FF1-F034-424C-A7E9-0CF1059B3A7C}" name="Distribution Type" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{41A11BA2-CB19-4A3D-BAB4-C7ABCBD3E30F}" name="Parameter 1" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{648D385E-E212-43CC-A8AA-53DDD8BD0428}" name="Parameter 2" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{A336D93E-1EE2-4808-98BA-CB978FBE172A}" name="Parameter 3" dataDxfId="46"/>
-    <tableColumn id="10" xr3:uid="{03178B46-AD0C-4482-9EC2-A764D5FA6F6C}" name="Parameter 4" dataDxfId="45"/>
-    <tableColumn id="11" xr3:uid="{EAD273F2-76B2-43C4-A1D7-A199E13BAD05}" name="Parameter 5" dataDxfId="44"/>
-    <tableColumn id="8" xr3:uid="{CA066BBA-6299-4A1A-A4D8-73F164A6F41D}" name="Parameter 6" dataDxfId="43"/>
-    <tableColumn id="15" xr3:uid="{F1632EF8-E0CB-4E7B-BEA5-E206CC27F984}" name="Lower Limit" dataDxfId="42"/>
-    <tableColumn id="16" xr3:uid="{4ED75AE2-55E4-419A-A9E6-19CC6C5896E9}" name="Upper Limit" dataDxfId="41"/>
-    <tableColumn id="17" xr3:uid="{D34421A0-FABD-4530-911F-6AAAC527E813}" name="Step" dataDxfId="40"/>
+    <tableColumn id="9" xr3:uid="{1735A646-077D-4A5C-8ABA-5E5552C83F8B}" name="Phase" dataDxfId="58"/>
+    <tableColumn id="20" xr3:uid="{004108F0-B585-4FC4-8E02-24F2EDB488C0}" name="Category" dataDxfId="57"/>
+    <tableColumn id="12" xr3:uid="{69E4893D-8A0F-46ED-8648-226BDC719B2B}" name="Name" dataDxfId="56"/>
+    <tableColumn id="14" xr3:uid="{A839FAC0-08F6-4AA7-96B8-39B9A47A057D}" name="Description" dataDxfId="55"/>
+    <tableColumn id="18" xr3:uid="{E0746BE3-6AD9-4082-A683-C57740CF7686}" name="Units" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{C6BD6FF1-F034-424C-A7E9-0CF1059B3A7C}" name="Distribution Type" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{41A11BA2-CB19-4A3D-BAB4-C7ABCBD3E30F}" name="Parameter 1" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{648D385E-E212-43CC-A8AA-53DDD8BD0428}" name="Parameter 2" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{A336D93E-1EE2-4808-98BA-CB978FBE172A}" name="Parameter 3" dataDxfId="50"/>
+    <tableColumn id="10" xr3:uid="{03178B46-AD0C-4482-9EC2-A764D5FA6F6C}" name="Parameter 4" dataDxfId="49"/>
+    <tableColumn id="11" xr3:uid="{EAD273F2-76B2-43C4-A1D7-A199E13BAD05}" name="Parameter 5" dataDxfId="48"/>
+    <tableColumn id="8" xr3:uid="{CA066BBA-6299-4A1A-A4D8-73F164A6F41D}" name="Parameter 6" dataDxfId="47"/>
+    <tableColumn id="15" xr3:uid="{F1632EF8-E0CB-4E7B-BEA5-E206CC27F984}" name="Lower Limit" dataDxfId="46"/>
+    <tableColumn id="16" xr3:uid="{4ED75AE2-55E4-419A-A9E6-19CC6C5896E9}" name="Upper Limit" dataDxfId="45"/>
+    <tableColumn id="17" xr3:uid="{D34421A0-FABD-4530-911F-6AAAC527E813}" name="Step" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{A9DDAA0B-EDE4-49CE-8D2A-53496C87AC6C}" name="Table156411" displayName="Table156411" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="35" tableBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{A9DDAA0B-EDE4-49CE-8D2A-53496C87AC6C}" name="Table156411" displayName="Table156411" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="39" tableBorderDxfId="38">
   <autoFilter ref="A1:O2" xr:uid="{96C1D83B-BC19-489F-9EB7-C4BD46C50E46}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{F67C5E8C-F091-4379-8FA4-1E0A53077B68}" name="Phase" dataDxfId="33"/>
-    <tableColumn id="20" xr3:uid="{F204C7B0-E561-4894-A461-ADBDC80CC735}" name="Category" dataDxfId="32"/>
-    <tableColumn id="12" xr3:uid="{30B72B9B-FF89-4E51-9A96-F8BE3F8041EA}" name="Name" dataDxfId="31"/>
-    <tableColumn id="14" xr3:uid="{DB30649B-C3C1-48BB-B0BA-3762B2EA3DA0}" name="Description" dataDxfId="30"/>
-    <tableColumn id="18" xr3:uid="{3421310D-974A-44DB-BC28-81CC179BFD51}" name="Units" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{A19068C9-4F23-4FE6-A45E-0F5BEA8C7692}" name="Distribution Type" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{8F241659-0C60-4FF4-9636-16A0AEB54DFB}" name="Parameter 1" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{AA2565DE-2D2D-4A58-BC4B-001FAEC9C3F0}" name="Parameter 2" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{CB9ADE6D-1E48-4ECA-BB61-8BFBE1C45E5E}" name="Parameter 3" dataDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{18EB0859-1F88-4B30-8715-88A124D91C9B}" name="Parameter 4" dataDxfId="24"/>
-    <tableColumn id="11" xr3:uid="{6D767472-81BC-463B-A56A-768C0F5A05A9}" name="Parameter 5" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{217B790C-1EC6-4F73-BB6C-25E35A9D36EE}" name="Parameter 6" dataDxfId="22"/>
-    <tableColumn id="15" xr3:uid="{D4DC6753-6BDE-420B-8E58-4073ED5E70CD}" name="Lower Limit" dataDxfId="21"/>
-    <tableColumn id="16" xr3:uid="{9E541401-2A45-4487-861E-572F306DBB90}" name="Upper Limit" dataDxfId="20"/>
-    <tableColumn id="17" xr3:uid="{222205B2-5966-4F6B-A5A4-259C62BDA43D}" name="Step" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{F67C5E8C-F091-4379-8FA4-1E0A53077B68}" name="Phase" dataDxfId="37"/>
+    <tableColumn id="20" xr3:uid="{F204C7B0-E561-4894-A461-ADBDC80CC735}" name="Category" dataDxfId="36"/>
+    <tableColumn id="12" xr3:uid="{30B72B9B-FF89-4E51-9A96-F8BE3F8041EA}" name="Name" dataDxfId="35"/>
+    <tableColumn id="14" xr3:uid="{DB30649B-C3C1-48BB-B0BA-3762B2EA3DA0}" name="Description" dataDxfId="34"/>
+    <tableColumn id="18" xr3:uid="{3421310D-974A-44DB-BC28-81CC179BFD51}" name="Units" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{A19068C9-4F23-4FE6-A45E-0F5BEA8C7692}" name="Distribution Type" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{8F241659-0C60-4FF4-9636-16A0AEB54DFB}" name="Parameter 1" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{AA2565DE-2D2D-4A58-BC4B-001FAEC9C3F0}" name="Parameter 2" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{CB9ADE6D-1E48-4ECA-BB61-8BFBE1C45E5E}" name="Parameter 3" dataDxfId="29"/>
+    <tableColumn id="10" xr3:uid="{18EB0859-1F88-4B30-8715-88A124D91C9B}" name="Parameter 4" dataDxfId="28"/>
+    <tableColumn id="11" xr3:uid="{6D767472-81BC-463B-A56A-768C0F5A05A9}" name="Parameter 5" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{217B790C-1EC6-4F73-BB6C-25E35A9D36EE}" name="Parameter 6" dataDxfId="26"/>
+    <tableColumn id="15" xr3:uid="{D4DC6753-6BDE-420B-8E58-4073ED5E70CD}" name="Lower Limit" dataDxfId="25"/>
+    <tableColumn id="16" xr3:uid="{9E541401-2A45-4487-861E-572F306DBB90}" name="Upper Limit" dataDxfId="24"/>
+    <tableColumn id="17" xr3:uid="{222205B2-5966-4F6B-A5A4-259C62BDA43D}" name="Step" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1C65CEB6-4F7A-4FD3-92D1-32B0AC0529C7}" name="Table15645" displayName="Table15645" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1C65CEB6-4F7A-4FD3-92D1-32B0AC0529C7}" name="Table15645" displayName="Table15645" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="20" tableBorderDxfId="19">
   <autoFilter ref="A1:O2" xr:uid="{CE70FAE3-DAD6-40A6-BCCE-F46A2CDA0980}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{A5634D1E-7F69-4A8B-9B2C-E544A100BE0B}" name="Phase" dataDxfId="14"/>
-    <tableColumn id="22" xr3:uid="{DF0A5598-36C6-480A-8445-5264CD38D6AE}" name="Category" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{322396A3-5A20-4A3E-8F7B-F97F31E5B741}" name="Name" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{1910CF64-CF8F-4994-BC1B-F27FE4E216E6}" name="Description" dataDxfId="11"/>
-    <tableColumn id="18" xr3:uid="{211B9116-478A-42BC-BFD9-0A2AA2AD39A9}" name="Units" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{ABD6291E-7951-4F95-9FF4-C5A1FC0AAC06}" name="Distribution Type" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{ECC3B9FC-E4AE-4AD1-BF4C-89FE38983ABB}" name="Parameter 1" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{8FC5359B-BA7A-46D2-B091-D9665C585235}" name="Parameter 2" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{3BDDE353-FD4F-45F2-8B7C-5F7D6E0D347D}" name="Parameter 3" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{701C65B5-1C54-4F3C-90E2-A67B32AB1876}" name="Parameter 4" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{A8EE834B-F323-4C30-8E59-AEDA8B9E2A61}" name="Parameter 5" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{240B8AE3-DEF4-4C61-BF40-2515EA4A4DDB}" name="Parameter 6" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{5D6076C4-791B-4994-9665-C628F9AE62B7}" name="Lower Limit" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{D06B2878-4A23-45AF-8278-C825D6961D31}" name="Upper Limit" dataDxfId="1"/>
-    <tableColumn id="17" xr3:uid="{54CBA85E-0128-4FD6-8F0E-932C4E402C1C}" name="Step" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{A5634D1E-7F69-4A8B-9B2C-E544A100BE0B}" name="Phase" dataDxfId="18"/>
+    <tableColumn id="22" xr3:uid="{DF0A5598-36C6-480A-8445-5264CD38D6AE}" name="Category" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{322396A3-5A20-4A3E-8F7B-F97F31E5B741}" name="Name" dataDxfId="16"/>
+    <tableColumn id="14" xr3:uid="{1910CF64-CF8F-4994-BC1B-F27FE4E216E6}" name="Description" dataDxfId="15"/>
+    <tableColumn id="18" xr3:uid="{211B9116-478A-42BC-BFD9-0A2AA2AD39A9}" name="Units" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{ABD6291E-7951-4F95-9FF4-C5A1FC0AAC06}" name="Distribution Type" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{ECC3B9FC-E4AE-4AD1-BF4C-89FE38983ABB}" name="Parameter 1" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{8FC5359B-BA7A-46D2-B091-D9665C585235}" name="Parameter 2" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{3BDDE353-FD4F-45F2-8B7C-5F7D6E0D347D}" name="Parameter 3" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{701C65B5-1C54-4F3C-90E2-A67B32AB1876}" name="Parameter 4" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{A8EE834B-F323-4C30-8E59-AEDA8B9E2A61}" name="Parameter 5" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{240B8AE3-DEF4-4C61-BF40-2515EA4A4DDB}" name="Parameter 6" dataDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{5D6076C4-791B-4994-9665-C628F9AE62B7}" name="Lower Limit" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{D06B2878-4A23-45AF-8278-C825D6961D31}" name="Upper Limit" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{54CBA85E-0128-4FD6-8F0E-932C4E402C1C}" name="Step" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15" displayName="Table15" ref="A1:O32" totalsRowShown="0" tableBorderDxfId="393">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15" displayName="Table15" ref="A1:O32" totalsRowShown="0" tableBorderDxfId="397">
   <autoFilter ref="A1:O32" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Phase" dataDxfId="392"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Category" dataDxfId="391"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="390"/>
-    <tableColumn id="10" xr3:uid="{8EBBFD49-190C-4C2F-A6BC-0598AAC3E788}" name="Description" dataDxfId="389"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Units" dataDxfId="388"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Distribution Type" dataDxfId="387"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Parameter 1" dataDxfId="386"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Parameter 2" dataDxfId="385"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Parameter 3" dataDxfId="384"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Parameter 4" dataDxfId="383"/>
-    <tableColumn id="14" xr3:uid="{E54D398D-B732-4333-A3F2-2EBD48BAA48B}" name="Parameter 5" dataDxfId="382"/>
-    <tableColumn id="15" xr3:uid="{47B382D4-92A3-4B8C-9C52-0458EA4788B1}" name="Parameter 6" dataDxfId="381"/>
-    <tableColumn id="11" xr3:uid="{BD4375F0-63E9-45EC-BE2E-338374C10F8B}" name="Lower Limit" dataDxfId="380"/>
-    <tableColumn id="12" xr3:uid="{E3D45A75-803F-48B4-B112-11C4C63E6D6F}" name="Upper Limit" dataDxfId="379"/>
-    <tableColumn id="13" xr3:uid="{FFEC12A7-FD01-4D8C-85CF-A25BD15B0829}" name="Step" dataDxfId="378"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Phase" dataDxfId="396"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Category" dataDxfId="395"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="394"/>
+    <tableColumn id="10" xr3:uid="{8EBBFD49-190C-4C2F-A6BC-0598AAC3E788}" name="Description" dataDxfId="393"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Units" dataDxfId="392"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Distribution Type" dataDxfId="391"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Parameter 1" dataDxfId="390"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Parameter 2" dataDxfId="389"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Parameter 3" dataDxfId="388"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Parameter 4" dataDxfId="387"/>
+    <tableColumn id="14" xr3:uid="{E54D398D-B732-4333-A3F2-2EBD48BAA48B}" name="Parameter 5" dataDxfId="386"/>
+    <tableColumn id="15" xr3:uid="{47B382D4-92A3-4B8C-9C52-0458EA4788B1}" name="Parameter 6" dataDxfId="385"/>
+    <tableColumn id="11" xr3:uid="{BD4375F0-63E9-45EC-BE2E-338374C10F8B}" name="Lower Limit" dataDxfId="384"/>
+    <tableColumn id="12" xr3:uid="{E3D45A75-803F-48B4-B112-11C4C63E6D6F}" name="Upper Limit" dataDxfId="383"/>
+    <tableColumn id="13" xr3:uid="{FFEC12A7-FD01-4D8C-85CF-A25BD15B0829}" name="Step" dataDxfId="382"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table157" displayName="Table157" ref="A1:O26" totalsRowShown="0" tableBorderDxfId="362">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table157" displayName="Table157" ref="A1:O26" totalsRowShown="0" tableBorderDxfId="366">
   <autoFilter ref="A1:O26" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Phase" dataDxfId="361"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Category" dataDxfId="360"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="359"/>
-    <tableColumn id="10" xr3:uid="{2D3DA962-F373-48F5-BD94-00CC27106A46}" name="Description" dataDxfId="358"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="357"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Distribution Type" dataDxfId="356"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Parameter 1" dataDxfId="355"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Parameter 2" dataDxfId="354"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Parameter 3" dataDxfId="353"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Parameter 4" dataDxfId="352"/>
-    <tableColumn id="14" xr3:uid="{5A98E335-B701-4CC9-9D03-A85D24786F3B}" name="Parameter 5" dataDxfId="351"/>
-    <tableColumn id="15" xr3:uid="{79377D49-ED29-41CF-AC28-FD408018808C}" name="Parameter 6" dataDxfId="350"/>
-    <tableColumn id="11" xr3:uid="{FF818C38-99D8-4486-B25F-2B94B62F77AF}" name="Lower Limit" dataDxfId="349"/>
-    <tableColumn id="12" xr3:uid="{8C44E4B8-6916-4798-9055-589FE4E4C903}" name="Upper Limit" dataDxfId="348"/>
-    <tableColumn id="13" xr3:uid="{8266E46A-7EC0-42D8-91D3-D2DC1B4352DE}" name="Step" dataDxfId="347"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Phase" dataDxfId="365"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Category" dataDxfId="364"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="363"/>
+    <tableColumn id="10" xr3:uid="{2D3DA962-F373-48F5-BD94-00CC27106A46}" name="Description" dataDxfId="362"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="361"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Distribution Type" dataDxfId="360"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Parameter 1" dataDxfId="359"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Parameter 2" dataDxfId="358"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Parameter 3" dataDxfId="357"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Parameter 4" dataDxfId="356"/>
+    <tableColumn id="14" xr3:uid="{5A98E335-B701-4CC9-9D03-A85D24786F3B}" name="Parameter 5" dataDxfId="355"/>
+    <tableColumn id="15" xr3:uid="{79377D49-ED29-41CF-AC28-FD408018808C}" name="Parameter 6" dataDxfId="354"/>
+    <tableColumn id="11" xr3:uid="{FF818C38-99D8-4486-B25F-2B94B62F77AF}" name="Lower Limit" dataDxfId="353"/>
+    <tableColumn id="12" xr3:uid="{8C44E4B8-6916-4798-9055-589FE4E4C903}" name="Upper Limit" dataDxfId="352"/>
+    <tableColumn id="13" xr3:uid="{8266E46A-7EC0-42D8-91D3-D2DC1B4352DE}" name="Step" dataDxfId="351"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1579" displayName="Table1579" ref="A1:O24" totalsRowShown="0" headerRowBorderDxfId="336" tableBorderDxfId="335">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1579" displayName="Table1579" ref="A1:O24" totalsRowShown="0" headerRowBorderDxfId="340" tableBorderDxfId="339">
   <autoFilter ref="A1:O24" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Phase" dataDxfId="334"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Category" dataDxfId="333"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name" dataDxfId="332"/>
-    <tableColumn id="10" xr3:uid="{A40104D1-3BF7-4068-8777-3D61F27973C1}" name="Description" dataDxfId="331"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Units" dataDxfId="330"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Distribution Type" dataDxfId="329"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Parameter 1" dataDxfId="328"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Parameter 2" dataDxfId="327"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Parameter 3" dataDxfId="326"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Parameter 4" dataDxfId="325"/>
-    <tableColumn id="14" xr3:uid="{77E616D7-C540-4C6C-A01C-31C8ADF35FBE}" name="Parameter 5" dataDxfId="324"/>
-    <tableColumn id="15" xr3:uid="{68C28D25-E41A-4D3D-A794-809A12A02364}" name="Parameter 6" dataDxfId="323"/>
-    <tableColumn id="11" xr3:uid="{83552614-5368-48EE-AE65-AA7B101E55EF}" name="Lower Limit" dataDxfId="322"/>
-    <tableColumn id="12" xr3:uid="{98998298-F4B1-4980-B79C-0BF0D0D59028}" name="Upper Limit" dataDxfId="321"/>
-    <tableColumn id="13" xr3:uid="{8E3814A1-C526-4157-B0D9-1258E47ACA45}" name="Step" dataDxfId="320"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Phase" dataDxfId="338"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Category" dataDxfId="337"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name" dataDxfId="336"/>
+    <tableColumn id="10" xr3:uid="{A40104D1-3BF7-4068-8777-3D61F27973C1}" name="Description" dataDxfId="335"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Units" dataDxfId="334"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Distribution Type" dataDxfId="333"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Parameter 1" dataDxfId="332"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Parameter 2" dataDxfId="331"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Parameter 3" dataDxfId="330"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Parameter 4" dataDxfId="329"/>
+    <tableColumn id="14" xr3:uid="{77E616D7-C540-4C6C-A01C-31C8ADF35FBE}" name="Parameter 5" dataDxfId="328"/>
+    <tableColumn id="15" xr3:uid="{68C28D25-E41A-4D3D-A794-809A12A02364}" name="Parameter 6" dataDxfId="327"/>
+    <tableColumn id="11" xr3:uid="{83552614-5368-48EE-AE65-AA7B101E55EF}" name="Lower Limit" dataDxfId="326"/>
+    <tableColumn id="12" xr3:uid="{98998298-F4B1-4980-B79C-0BF0D0D59028}" name="Upper Limit" dataDxfId="325"/>
+    <tableColumn id="13" xr3:uid="{8E3814A1-C526-4157-B0D9-1258E47ACA45}" name="Step" dataDxfId="324"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{8CFD0B9C-5C13-4227-BBD4-CC3E2EA79A0D}" name="Table1520" displayName="Table1520" ref="A1:O32" totalsRowShown="0" tableBorderDxfId="312">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{8CFD0B9C-5C13-4227-BBD4-CC3E2EA79A0D}" name="Table1520" displayName="Table1520" ref="A1:O32" totalsRowShown="0" tableBorderDxfId="316">
   <autoFilter ref="A1:O32" xr:uid="{8CFD0B9C-5C13-4227-BBD4-CC3E2EA79A0D}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{F3EBEF0A-C49D-4631-895D-C0AA8DE0387C}" name="Phase" dataDxfId="311"/>
-    <tableColumn id="1" xr3:uid="{3248CADE-36E9-4F6B-8C04-EAB19C6554F4}" name="Category" dataDxfId="310"/>
-    <tableColumn id="2" xr3:uid="{51D878BC-C331-482D-9463-0725B579E498}" name="Name" dataDxfId="309"/>
-    <tableColumn id="10" xr3:uid="{85E2341D-9337-4CD8-8015-CFEEC676EF80}" name="Description" dataDxfId="308"/>
-    <tableColumn id="3" xr3:uid="{352CC463-6E94-472E-9C21-4F628D3132B5}" name="Units" dataDxfId="307"/>
-    <tableColumn id="4" xr3:uid="{03A26550-CFC5-4337-8C74-285910A13C88}" name="Distribution Type" dataDxfId="306"/>
-    <tableColumn id="5" xr3:uid="{3B6C3336-ACCA-40B1-8EAD-3C1126611C06}" name="Parameter 1" dataDxfId="305"/>
-    <tableColumn id="6" xr3:uid="{F8658D67-C2A3-41F0-BC30-7C1BC44088E6}" name="Parameter 2" dataDxfId="304"/>
-    <tableColumn id="7" xr3:uid="{CE81C17A-BCB8-46E7-8DEC-84C04A43C420}" name="Parameter 3" dataDxfId="303"/>
-    <tableColumn id="8" xr3:uid="{C6458EC6-C037-4BD8-B16F-CB6126C12426}" name="Parameter 4" dataDxfId="302"/>
-    <tableColumn id="14" xr3:uid="{952AB6AA-B2DE-4020-8F81-D936468E97C0}" name="Parameter 5" dataDxfId="301"/>
-    <tableColumn id="15" xr3:uid="{D3B4E926-32F3-407C-BA36-D0E7215FA966}" name="Parameter 6" dataDxfId="300"/>
-    <tableColumn id="11" xr3:uid="{00B748A6-A24A-4C90-8CFE-84590E669D75}" name="Lower Limit" dataDxfId="299"/>
-    <tableColumn id="12" xr3:uid="{13DEB792-693B-402C-BCC0-5F1CD3F37B24}" name="Upper Limit" dataDxfId="298"/>
-    <tableColumn id="13" xr3:uid="{4C2918D4-3BEE-42B5-ADE1-FF74A8BC4482}" name="Step" dataDxfId="297"/>
+    <tableColumn id="9" xr3:uid="{F3EBEF0A-C49D-4631-895D-C0AA8DE0387C}" name="Phase" dataDxfId="315"/>
+    <tableColumn id="1" xr3:uid="{3248CADE-36E9-4F6B-8C04-EAB19C6554F4}" name="Category" dataDxfId="314"/>
+    <tableColumn id="2" xr3:uid="{51D878BC-C331-482D-9463-0725B579E498}" name="Name" dataDxfId="313"/>
+    <tableColumn id="10" xr3:uid="{85E2341D-9337-4CD8-8015-CFEEC676EF80}" name="Description" dataDxfId="312"/>
+    <tableColumn id="3" xr3:uid="{352CC463-6E94-472E-9C21-4F628D3132B5}" name="Units" dataDxfId="311"/>
+    <tableColumn id="4" xr3:uid="{03A26550-CFC5-4337-8C74-285910A13C88}" name="Distribution Type" dataDxfId="310"/>
+    <tableColumn id="5" xr3:uid="{3B6C3336-ACCA-40B1-8EAD-3C1126611C06}" name="Parameter 1" dataDxfId="309"/>
+    <tableColumn id="6" xr3:uid="{F8658D67-C2A3-41F0-BC30-7C1BC44088E6}" name="Parameter 2" dataDxfId="308"/>
+    <tableColumn id="7" xr3:uid="{CE81C17A-BCB8-46E7-8DEC-84C04A43C420}" name="Parameter 3" dataDxfId="307"/>
+    <tableColumn id="8" xr3:uid="{C6458EC6-C037-4BD8-B16F-CB6126C12426}" name="Parameter 4" dataDxfId="306"/>
+    <tableColumn id="14" xr3:uid="{952AB6AA-B2DE-4020-8F81-D936468E97C0}" name="Parameter 5" dataDxfId="305"/>
+    <tableColumn id="15" xr3:uid="{D3B4E926-32F3-407C-BA36-D0E7215FA966}" name="Parameter 6" dataDxfId="304"/>
+    <tableColumn id="11" xr3:uid="{00B748A6-A24A-4C90-8CFE-84590E669D75}" name="Lower Limit" dataDxfId="303"/>
+    <tableColumn id="12" xr3:uid="{13DEB792-693B-402C-BCC0-5F1CD3F37B24}" name="Upper Limit" dataDxfId="302"/>
+    <tableColumn id="13" xr3:uid="{4C2918D4-3BEE-42B5-ADE1-FF74A8BC4482}" name="Step" dataDxfId="301"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{7330A672-C943-4362-821B-755573408116}" name="Table1521" displayName="Table1521" ref="A1:O34" totalsRowShown="0" tableBorderDxfId="287">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{7330A672-C943-4362-821B-755573408116}" name="Table1521" displayName="Table1521" ref="A1:O34" totalsRowShown="0" tableBorderDxfId="291">
   <autoFilter ref="A1:O34" xr:uid="{7330A672-C943-4362-821B-755573408116}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{B133B9E4-820A-4680-BCDD-704A3C728372}" name="Phase" dataDxfId="286"/>
-    <tableColumn id="1" xr3:uid="{0C52E358-F746-4AB6-A186-E9F57DC3488C}" name="Category" dataDxfId="285"/>
-    <tableColumn id="2" xr3:uid="{3EB687B2-94CD-4468-838E-53D1ED3E92AD}" name="Name" dataDxfId="284"/>
-    <tableColumn id="10" xr3:uid="{48F735C1-6CD8-47D1-8F20-910C557D8DE5}" name="Description" dataDxfId="283"/>
-    <tableColumn id="3" xr3:uid="{D0BD7EC3-8CC3-442D-B9BD-BE7C714173ED}" name="Units" dataDxfId="282"/>
-    <tableColumn id="4" xr3:uid="{3AA698E5-4D28-4598-A0BE-C99F25507CDF}" name="Distribution Type" dataDxfId="281"/>
-    <tableColumn id="5" xr3:uid="{25A9745D-9B26-408E-A43E-16235B7DFC6C}" name="Parameter 1" dataDxfId="280"/>
-    <tableColumn id="6" xr3:uid="{CA609044-DDDF-4C5D-9F10-C588B31C94B0}" name="Parameter 2" dataDxfId="279"/>
-    <tableColumn id="7" xr3:uid="{CCB86206-76D0-4ABB-A2F9-AE89D61B8D45}" name="Parameter 3" dataDxfId="278"/>
-    <tableColumn id="8" xr3:uid="{9DDAD0C7-7150-4C7A-8CC1-7CA55268D2F2}" name="Parameter 4" dataDxfId="277"/>
-    <tableColumn id="14" xr3:uid="{C33C5E5C-1FFC-4C5F-9F33-FD7D79906B77}" name="Parameter 5" dataDxfId="276"/>
-    <tableColumn id="15" xr3:uid="{4EC6D868-8CE7-424C-9953-B01CAA077D51}" name="Parameter 6" dataDxfId="275"/>
-    <tableColumn id="11" xr3:uid="{C8797205-E1CA-4AD8-BE1C-EBCFC768BE51}" name="Lower Limit" dataDxfId="274"/>
-    <tableColumn id="12" xr3:uid="{2E665777-FC21-4123-AC7B-1763610C7AF4}" name="Upper Limit" dataDxfId="273"/>
-    <tableColumn id="13" xr3:uid="{0283BE4B-5056-4073-98BD-609D701ACEA2}" name="Step" dataDxfId="272"/>
+    <tableColumn id="9" xr3:uid="{B133B9E4-820A-4680-BCDD-704A3C728372}" name="Phase" dataDxfId="290"/>
+    <tableColumn id="1" xr3:uid="{0C52E358-F746-4AB6-A186-E9F57DC3488C}" name="Category" dataDxfId="289"/>
+    <tableColumn id="2" xr3:uid="{3EB687B2-94CD-4468-838E-53D1ED3E92AD}" name="Name" dataDxfId="288"/>
+    <tableColumn id="10" xr3:uid="{48F735C1-6CD8-47D1-8F20-910C557D8DE5}" name="Description" dataDxfId="287"/>
+    <tableColumn id="3" xr3:uid="{D0BD7EC3-8CC3-442D-B9BD-BE7C714173ED}" name="Units" dataDxfId="286"/>
+    <tableColumn id="4" xr3:uid="{3AA698E5-4D28-4598-A0BE-C99F25507CDF}" name="Distribution Type" dataDxfId="285"/>
+    <tableColumn id="5" xr3:uid="{25A9745D-9B26-408E-A43E-16235B7DFC6C}" name="Parameter 1" dataDxfId="284"/>
+    <tableColumn id="6" xr3:uid="{CA609044-DDDF-4C5D-9F10-C588B31C94B0}" name="Parameter 2" dataDxfId="283"/>
+    <tableColumn id="7" xr3:uid="{CCB86206-76D0-4ABB-A2F9-AE89D61B8D45}" name="Parameter 3" dataDxfId="282"/>
+    <tableColumn id="8" xr3:uid="{9DDAD0C7-7150-4C7A-8CC1-7CA55268D2F2}" name="Parameter 4" dataDxfId="281"/>
+    <tableColumn id="14" xr3:uid="{C33C5E5C-1FFC-4C5F-9F33-FD7D79906B77}" name="Parameter 5" dataDxfId="280"/>
+    <tableColumn id="15" xr3:uid="{4EC6D868-8CE7-424C-9953-B01CAA077D51}" name="Parameter 6" dataDxfId="279"/>
+    <tableColumn id="11" xr3:uid="{C8797205-E1CA-4AD8-BE1C-EBCFC768BE51}" name="Lower Limit" dataDxfId="278"/>
+    <tableColumn id="12" xr3:uid="{2E665777-FC21-4123-AC7B-1763610C7AF4}" name="Upper Limit" dataDxfId="277"/>
+    <tableColumn id="13" xr3:uid="{0283BE4B-5056-4073-98BD-609D701ACEA2}" name="Step" dataDxfId="276"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table15793" displayName="Table15793" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="267" tableBorderDxfId="266">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table15793" displayName="Table15793" ref="A1:O2" totalsRowShown="0" headerRowBorderDxfId="271" tableBorderDxfId="270">
   <autoFilter ref="A1:O2" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Phase" dataDxfId="265"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Category" dataDxfId="264"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Name" dataDxfId="263"/>
-    <tableColumn id="10" xr3:uid="{4482773E-AA48-4795-9A9F-10283D12A976}" name="Description" dataDxfId="262"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Units" dataDxfId="261"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Distribution Type" dataDxfId="260"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Parameter 1" dataDxfId="259"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Parameter 2" dataDxfId="258"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Parameter 3" dataDxfId="257"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Parameter 4" dataDxfId="256"/>
-    <tableColumn id="14" xr3:uid="{41E058E9-8EB6-430E-BC58-82195628B7D1}" name="Parameter 5" dataDxfId="255"/>
-    <tableColumn id="15" xr3:uid="{1CA16974-E252-4655-813D-3FC48E8CCF45}" name="Parameter 6" dataDxfId="254"/>
-    <tableColumn id="11" xr3:uid="{0ED7EC4B-FD74-44E3-B1E6-428C431FDA88}" name="Lower Limit" dataDxfId="253"/>
-    <tableColumn id="12" xr3:uid="{4CA3754D-692A-40C0-BCC5-14D0E3AAF144}" name="Upper Limit" dataDxfId="252"/>
-    <tableColumn id="13" xr3:uid="{D4791B88-6435-44AE-9946-77D4E8CB6EA8}" name="Step" dataDxfId="251"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Phase" dataDxfId="269"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Category" dataDxfId="268"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Name" dataDxfId="267"/>
+    <tableColumn id="10" xr3:uid="{4482773E-AA48-4795-9A9F-10283D12A976}" name="Description" dataDxfId="266"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Units" dataDxfId="265"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Distribution Type" dataDxfId="264"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Parameter 1" dataDxfId="263"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Parameter 2" dataDxfId="262"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Parameter 3" dataDxfId="261"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Parameter 4" dataDxfId="260"/>
+    <tableColumn id="14" xr3:uid="{41E058E9-8EB6-430E-BC58-82195628B7D1}" name="Parameter 5" dataDxfId="259"/>
+    <tableColumn id="15" xr3:uid="{1CA16974-E252-4655-813D-3FC48E8CCF45}" name="Parameter 6" dataDxfId="258"/>
+    <tableColumn id="11" xr3:uid="{0ED7EC4B-FD74-44E3-B1E6-428C431FDA88}" name="Lower Limit" dataDxfId="257"/>
+    <tableColumn id="12" xr3:uid="{4CA3754D-692A-40C0-BCC5-14D0E3AAF144}" name="Upper Limit" dataDxfId="256"/>
+    <tableColumn id="13" xr3:uid="{D4791B88-6435-44AE-9946-77D4E8CB6EA8}" name="Step" dataDxfId="255"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157910" displayName="Table157910" ref="A1:O31" totalsRowShown="0" headerRowBorderDxfId="240" tableBorderDxfId="239">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157910" displayName="Table157910" ref="A1:O31" totalsRowShown="0" headerRowBorderDxfId="244" tableBorderDxfId="243">
   <autoFilter ref="A1:O31" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J2">
     <sortCondition ref="B1:B2"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="Phase" dataDxfId="238"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Category" dataDxfId="237"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Name" dataDxfId="236"/>
-    <tableColumn id="10" xr3:uid="{3AFE3909-1CDD-46E0-8677-569A824534FB}" name="Description" dataDxfId="235"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Units" dataDxfId="234"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Distribution Type" dataDxfId="233"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Parameter 1" dataDxfId="232"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Parameter 2" dataDxfId="231"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Parameter 3" dataDxfId="230"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Parameter 4" dataDxfId="229"/>
-    <tableColumn id="14" xr3:uid="{8991E047-B1B0-4B74-A5AA-45E689F51874}" name="Parameter 5" dataDxfId="228"/>
-    <tableColumn id="15" xr3:uid="{A25E7AA9-7C49-405C-8326-53EA8C994FFB}" name="Parameter 6" dataDxfId="227"/>
-    <tableColumn id="11" xr3:uid="{08FFB9BF-C539-434A-A2F4-C19873D3AB3E}" name="Lower Limit" dataDxfId="226"/>
-    <tableColumn id="12" xr3:uid="{CEDB540F-344B-4D49-8CD6-9F7746873840}" name="Upper Limit" dataDxfId="225"/>
-    <tableColumn id="13" xr3:uid="{4B3E9A2A-7D0A-4F2D-B694-DB4D2C83BA0A}" name="Step" dataDxfId="224"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="Phase" dataDxfId="242"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Category" dataDxfId="241"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Name" dataDxfId="240"/>
+    <tableColumn id="10" xr3:uid="{3AFE3909-1CDD-46E0-8677-569A824534FB}" name="Description" dataDxfId="239"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Units" dataDxfId="238"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Distribution Type" dataDxfId="237"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Parameter 1" dataDxfId="236"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Parameter 2" dataDxfId="235"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Parameter 3" dataDxfId="234"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Parameter 4" dataDxfId="233"/>
+    <tableColumn id="14" xr3:uid="{8991E047-B1B0-4B74-A5AA-45E689F51874}" name="Parameter 5" dataDxfId="232"/>
+    <tableColumn id="15" xr3:uid="{A25E7AA9-7C49-405C-8326-53EA8C994FFB}" name="Parameter 6" dataDxfId="231"/>
+    <tableColumn id="11" xr3:uid="{08FFB9BF-C539-434A-A2F4-C19873D3AB3E}" name="Lower Limit" dataDxfId="230"/>
+    <tableColumn id="12" xr3:uid="{CEDB540F-344B-4D49-8CD6-9F7746873840}" name="Upper Limit" dataDxfId="229"/>
+    <tableColumn id="13" xr3:uid="{4B3E9A2A-7D0A-4F2D-B694-DB4D2C83BA0A}" name="Step" dataDxfId="228"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{386DF0A0-F564-45BE-827C-AB9E514445DE}" name="Table15798" displayName="Table15798" ref="A1:O19" totalsRowShown="0" headerRowBorderDxfId="220" tableBorderDxfId="219">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{386DF0A0-F564-45BE-827C-AB9E514445DE}" name="Table15798" displayName="Table15798" ref="A1:O19" totalsRowShown="0" headerRowBorderDxfId="224" tableBorderDxfId="223">
   <autoFilter ref="A1:O19" xr:uid="{20F9ED21-B94D-45D6-AD09-CA10F84B0D78}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{105D3C93-B71D-4BBE-A32C-8D325548C693}" name="Phase" dataDxfId="218"/>
-    <tableColumn id="1" xr3:uid="{F1853721-4335-498C-9A5F-F0BFEA4A2463}" name="Category" dataDxfId="217"/>
-    <tableColumn id="2" xr3:uid="{AE781E6F-7188-4759-9A88-06BC1C8C5519}" name="Name" dataDxfId="216"/>
-    <tableColumn id="10" xr3:uid="{102C3C27-81C3-48A8-A777-CFE96E393517}" name="Description" dataDxfId="215"/>
-    <tableColumn id="3" xr3:uid="{E8847F97-841C-43AA-B4C5-86A72C3D6D42}" name="Units" dataDxfId="214"/>
-    <tableColumn id="4" xr3:uid="{528D811A-B6F9-4674-AECE-ABC6F4ABB203}" name="Distribution Type" dataDxfId="213"/>
-    <tableColumn id="5" xr3:uid="{4551144E-FB04-473E-9929-E8A70CBC3A3C}" name="Parameter 1" dataDxfId="212"/>
-    <tableColumn id="6" xr3:uid="{21380B39-BE02-443C-8CD5-0C8659870D2C}" name="Parameter 2" dataDxfId="211"/>
-    <tableColumn id="7" xr3:uid="{D78AA71B-625F-4180-9197-F2EA9670D953}" name="Parameter 3" dataDxfId="210"/>
-    <tableColumn id="8" xr3:uid="{6BD21F32-4FF7-49FF-B1AA-3A5B27396AB4}" name="Parameter 4" dataDxfId="209"/>
-    <tableColumn id="14" xr3:uid="{F6AEC084-5785-4EE8-B9B9-3BF7A867A002}" name="Parameter 5" dataDxfId="208"/>
-    <tableColumn id="15" xr3:uid="{A85885A3-48F2-402A-A077-C70E7FB7984C}" name="Parameter 6" dataDxfId="207"/>
-    <tableColumn id="11" xr3:uid="{77F976B7-4356-41CD-9396-34DE1445193E}" name="Lower Limit" dataDxfId="206"/>
-    <tableColumn id="12" xr3:uid="{750C57B1-4D14-4E06-BDEF-5018AC9C0418}" name="Upper Limit" dataDxfId="205"/>
-    <tableColumn id="13" xr3:uid="{E0FF3252-91C6-49AA-A0EB-449B8D9DD283}" name="Step" dataDxfId="204"/>
+    <tableColumn id="9" xr3:uid="{105D3C93-B71D-4BBE-A32C-8D325548C693}" name="Phase" dataDxfId="222"/>
+    <tableColumn id="1" xr3:uid="{F1853721-4335-498C-9A5F-F0BFEA4A2463}" name="Category" dataDxfId="221"/>
+    <tableColumn id="2" xr3:uid="{AE781E6F-7188-4759-9A88-06BC1C8C5519}" name="Name" dataDxfId="220"/>
+    <tableColumn id="10" xr3:uid="{102C3C27-81C3-48A8-A777-CFE96E393517}" name="Description" dataDxfId="219"/>
+    <tableColumn id="3" xr3:uid="{E8847F97-841C-43AA-B4C5-86A72C3D6D42}" name="Units" dataDxfId="218"/>
+    <tableColumn id="4" xr3:uid="{528D811A-B6F9-4674-AECE-ABC6F4ABB203}" name="Distribution Type" dataDxfId="217"/>
+    <tableColumn id="5" xr3:uid="{4551144E-FB04-473E-9929-E8A70CBC3A3C}" name="Parameter 1" dataDxfId="216"/>
+    <tableColumn id="6" xr3:uid="{21380B39-BE02-443C-8CD5-0C8659870D2C}" name="Parameter 2" dataDxfId="215"/>
+    <tableColumn id="7" xr3:uid="{D78AA71B-625F-4180-9197-F2EA9670D953}" name="Parameter 3" dataDxfId="214"/>
+    <tableColumn id="8" xr3:uid="{6BD21F32-4FF7-49FF-B1AA-3A5B27396AB4}" name="Parameter 4" dataDxfId="213"/>
+    <tableColumn id="14" xr3:uid="{F6AEC084-5785-4EE8-B9B9-3BF7A867A002}" name="Parameter 5" dataDxfId="212"/>
+    <tableColumn id="15" xr3:uid="{A85885A3-48F2-402A-A077-C70E7FB7984C}" name="Parameter 6" dataDxfId="211"/>
+    <tableColumn id="11" xr3:uid="{77F976B7-4356-41CD-9396-34DE1445193E}" name="Lower Limit" dataDxfId="210"/>
+    <tableColumn id="12" xr3:uid="{750C57B1-4D14-4E06-BDEF-5018AC9C0418}" name="Upper Limit" dataDxfId="209"/>
+    <tableColumn id="13" xr3:uid="{E0FF3252-91C6-49AA-A0EB-449B8D9DD283}" name="Step" dataDxfId="208"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8700,7 +8733,7 @@
         <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>152</v>
@@ -8732,20 +8765,20 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L2">
-    <cfRule type="expression" dxfId="271" priority="26">
+    <cfRule type="expression" dxfId="275" priority="26">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="270" priority="1">
+    <cfRule type="expression" dxfId="274" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="269" priority="2">
+    <cfRule type="expression" dxfId="273" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:L2">
-    <cfRule type="expression" dxfId="268" priority="129">
+    <cfRule type="expression" dxfId="272" priority="129">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8870,7 +8903,7 @@
         <v>45</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>157</v>
@@ -8907,7 +8940,7 @@
         <v>45</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>158</v>
@@ -8944,7 +8977,7 @@
         <v>45</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>159</v>
@@ -8981,10 +9014,10 @@
         <v>45</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>70</v>
@@ -9018,10 +9051,10 @@
         <v>45</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>70</v>
@@ -9055,10 +9088,10 @@
         <v>45</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>70</v>
@@ -9277,10 +9310,10 @@
         <v>45</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>70</v>
@@ -9314,10 +9347,10 @@
         <v>45</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>70</v>
@@ -9388,7 +9421,7 @@
         <v>45</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>162</v>
@@ -9462,7 +9495,7 @@
         <v>45</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>164</v>
@@ -9499,7 +9532,7 @@
         <v>45</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>187</v>
@@ -9536,13 +9569,13 @@
         <v>32</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>3</v>
@@ -9573,13 +9606,13 @@
         <v>32</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>3</v>
@@ -9758,7 +9791,7 @@
         <v>45</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>169</v>
@@ -9795,7 +9828,7 @@
         <v>45</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>170</v>
@@ -9832,7 +9865,7 @@
         <v>32</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>191</v>
@@ -9869,13 +9902,13 @@
         <v>45</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>3</v>
@@ -9906,13 +9939,13 @@
         <v>32</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F31" s="11" t="s">
         <v>3</v>
@@ -9938,50 +9971,50 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L6 G8:L31">
-    <cfRule type="expression" dxfId="250" priority="40">
+    <cfRule type="expression" dxfId="254" priority="40">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="249" priority="12">
+    <cfRule type="expression" dxfId="253" priority="12">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="248" priority="13">
+    <cfRule type="expression" dxfId="252" priority="13">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:L2 A3:L5 F23:F31 G23:L28 A23:E28 A16:L20 A9:L13">
-    <cfRule type="expression" dxfId="247" priority="139">
+    <cfRule type="expression" dxfId="251" priority="139">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:L14">
-    <cfRule type="expression" dxfId="246" priority="9">
+    <cfRule type="expression" dxfId="250" priority="9">
       <formula>ISBLANK($F14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:L15">
-    <cfRule type="expression" dxfId="245" priority="8">
+    <cfRule type="expression" dxfId="249" priority="8">
       <formula>ISBLANK($F15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:L6">
-    <cfRule type="expression" dxfId="244" priority="5">
+    <cfRule type="expression" dxfId="248" priority="5">
       <formula>ISBLANK($F6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:L8">
-    <cfRule type="expression" dxfId="243" priority="4">
+    <cfRule type="expression" dxfId="247" priority="4">
       <formula>ISBLANK($F8)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:L7">
-    <cfRule type="expression" dxfId="242" priority="2">
+    <cfRule type="expression" dxfId="246" priority="2">
       <formula>NOT((COLUMN(G7)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F7, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:L7">
-    <cfRule type="expression" dxfId="241" priority="1">
+    <cfRule type="expression" dxfId="245" priority="1">
       <formula>ISBLANK($F7)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10071,19 +10104,19 @@
         <v>100</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>242</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>245</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>210</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>193</v>
@@ -10105,16 +10138,16 @@
         <v>110</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>210</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>193</v>
@@ -10136,16 +10169,16 @@
         <v>109</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>193</v>
@@ -10167,16 +10200,16 @@
         <v>103</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>210</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>193</v>
@@ -10195,19 +10228,19 @@
         <v>100</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>210</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>193</v>
@@ -10229,16 +10262,16 @@
         <v>111</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>210</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>193</v>
@@ -10260,16 +10293,16 @@
         <v>112</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>210</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>193</v>
@@ -10291,16 +10324,16 @@
         <v>105</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>210</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>193</v>
@@ -10322,16 +10355,16 @@
         <v>113</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>210</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>193</v>
@@ -10350,19 +10383,19 @@
         <v>104</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>210</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G11" s="14" t="s">
         <v>193</v>
@@ -10381,19 +10414,19 @@
         <v>104</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>210</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G12" s="14" t="s">
         <v>193</v>
@@ -10415,16 +10448,16 @@
         <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>210</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G13" s="14" t="s">
         <v>193</v>
@@ -10443,19 +10476,19 @@
         <v>106</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>210</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G14" s="14" t="s">
         <v>193</v>
@@ -10477,16 +10510,16 @@
         <v>116</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>210</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G15" s="14" t="s">
         <v>193</v>
@@ -10508,16 +10541,16 @@
         <v>115</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>210</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G16" s="14" t="s">
         <v>193</v>
@@ -10539,16 +10572,16 @@
         <v>107</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>210</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>193</v>
@@ -10567,19 +10600,19 @@
         <v>106</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>210</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>193</v>
@@ -10598,19 +10631,19 @@
         <v>106</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>210</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G19" s="14" t="s">
         <v>193</v>
@@ -10626,15 +10659,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:L19">
-    <cfRule type="expression" dxfId="223" priority="8">
+    <cfRule type="expression" dxfId="227" priority="8">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A19">
-    <cfRule type="expression" dxfId="222" priority="6">
+    <cfRule type="expression" dxfId="226" priority="6">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="221" priority="7">
+    <cfRule type="expression" dxfId="225" priority="7">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10772,20 +10805,20 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L2">
-    <cfRule type="expression" dxfId="203" priority="3">
+    <cfRule type="expression" dxfId="207" priority="3">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:L2">
-    <cfRule type="expression" dxfId="202" priority="4">
+    <cfRule type="expression" dxfId="206" priority="4">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="201" priority="1">
+    <cfRule type="expression" dxfId="205" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="200" priority="2">
+    <cfRule type="expression" dxfId="204" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10910,20 +10943,20 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L2">
-    <cfRule type="expression" dxfId="182" priority="142">
+    <cfRule type="expression" dxfId="186" priority="142">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="181" priority="140">
+    <cfRule type="expression" dxfId="185" priority="140">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="180" priority="141">
+    <cfRule type="expression" dxfId="184" priority="141">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:L2">
-    <cfRule type="expression" dxfId="179" priority="143">
+    <cfRule type="expression" dxfId="183" priority="143">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11045,20 +11078,20 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L2">
-    <cfRule type="expression" dxfId="161" priority="17">
+    <cfRule type="expression" dxfId="165" priority="17">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="160" priority="15">
+    <cfRule type="expression" dxfId="164" priority="15">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="159" priority="16">
+    <cfRule type="expression" dxfId="163" priority="16">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:L2">
-    <cfRule type="expression" dxfId="158" priority="18">
+    <cfRule type="expression" dxfId="162" priority="18">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11181,20 +11214,20 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L2">
-    <cfRule type="expression" dxfId="140" priority="3">
+    <cfRule type="expression" dxfId="144" priority="3">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="139" priority="1">
+    <cfRule type="expression" dxfId="143" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="2">
+    <cfRule type="expression" dxfId="142" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:L2">
-    <cfRule type="expression" dxfId="137" priority="4">
+    <cfRule type="expression" dxfId="141" priority="4">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11316,20 +11349,20 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L2">
-    <cfRule type="expression" dxfId="119" priority="3">
+    <cfRule type="expression" dxfId="123" priority="3">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="118" priority="1">
+    <cfRule type="expression" dxfId="122" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="2">
+    <cfRule type="expression" dxfId="121" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:L2">
-    <cfRule type="expression" dxfId="116" priority="4">
+    <cfRule type="expression" dxfId="120" priority="4">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11452,12 +11485,12 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L2">
-    <cfRule type="expression" dxfId="98" priority="3">
+    <cfRule type="expression" dxfId="102" priority="3">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:L2">
-    <cfRule type="expression" dxfId="97" priority="4">
+    <cfRule type="expression" dxfId="101" priority="4">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11582,12 +11615,12 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L2">
-    <cfRule type="expression" dxfId="79" priority="71">
+    <cfRule type="expression" dxfId="83" priority="71">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2 B2:F2">
-    <cfRule type="expression" dxfId="78" priority="68">
+    <cfRule type="expression" dxfId="82" priority="68">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11654,7 +11687,7 @@
         <v>86</v>
       </c>
       <c r="J1" s="25" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -11694,7 +11727,7 @@
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
       <c r="J3" s="11" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -11788,7 +11821,7 @@
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
       <c r="J7" s="11" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -11809,7 +11842,7 @@
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
       <c r="J8" s="11" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -11830,7 +11863,7 @@
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
       <c r="J9" s="11" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -11884,18 +11917,18 @@
         <v>76</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B12" s="21">
         <v>1</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
@@ -12043,20 +12076,20 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L2">
-    <cfRule type="expression" dxfId="60" priority="3">
+    <cfRule type="expression" dxfId="64" priority="3">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="59" priority="1">
+    <cfRule type="expression" dxfId="63" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="2">
+    <cfRule type="expression" dxfId="62" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:L2">
-    <cfRule type="expression" dxfId="57" priority="4">
+    <cfRule type="expression" dxfId="61" priority="4">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12180,20 +12213,20 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L2">
-    <cfRule type="expression" dxfId="39" priority="84">
+    <cfRule type="expression" dxfId="43" priority="84">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="38" priority="82">
+    <cfRule type="expression" dxfId="42" priority="82">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="83">
+    <cfRule type="expression" dxfId="41" priority="83">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:L2">
-    <cfRule type="expression" dxfId="36" priority="85">
+    <cfRule type="expression" dxfId="40" priority="85">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12316,12 +12349,12 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L2">
-    <cfRule type="expression" dxfId="18" priority="3">
+    <cfRule type="expression" dxfId="22" priority="3">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:L2">
-    <cfRule type="expression" dxfId="17" priority="4">
+    <cfRule type="expression" dxfId="21" priority="4">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12810,25 +12843,25 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A2:L2 A8:L8 F3:L6 D3:D6 A3:B7">
-    <cfRule type="expression" dxfId="421" priority="138">
+    <cfRule type="expression" dxfId="425" priority="138">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="420" priority="139">
+    <cfRule type="expression" dxfId="424" priority="139">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C6 E3:E6">
-    <cfRule type="expression" dxfId="419" priority="5">
+    <cfRule type="expression" dxfId="423" priority="5">
       <formula>ISBLANK($F3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:L7">
-    <cfRule type="expression" dxfId="418" priority="1">
+    <cfRule type="expression" dxfId="422" priority="1">
       <formula>NOT((COLUMN(G7)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F7, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:L7">
-    <cfRule type="expression" dxfId="417" priority="2">
+    <cfRule type="expression" dxfId="421" priority="2">
       <formula>ISBLANK($F7)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12850,8 +12883,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13177,7 +13210,7 @@
         <v>45</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>175</v>
@@ -13251,7 +13284,7 @@
         <v>45</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>145</v>
@@ -13399,7 +13432,7 @@
         <v>32</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>148</v>
@@ -13510,13 +13543,13 @@
         <v>32</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>3</v>
@@ -13547,13 +13580,13 @@
         <v>32</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>3</v>
@@ -13584,13 +13617,13 @@
         <v>32</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>3</v>
@@ -13658,10 +13691,10 @@
         <v>32</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>220</v>
+        <v>314</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>214</v>
+        <v>315</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>211</v>
@@ -13670,7 +13703,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="14">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
@@ -13681,10 +13714,10 @@
         <v>0</v>
       </c>
       <c r="N22" s="14">
-        <v>10000</v>
+        <v>72</v>
       </c>
       <c r="O22" s="14">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -13698,10 +13731,10 @@
         <v>202</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F23" s="11" t="s">
         <v>3</v>
@@ -13732,13 +13765,13 @@
         <v>32</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F24" s="11" t="s">
         <v>3</v>
@@ -13769,13 +13802,13 @@
         <v>32</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>3</v>
@@ -13806,13 +13839,13 @@
         <v>32</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>3</v>
@@ -13843,13 +13876,13 @@
         <v>32</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>3</v>
@@ -13880,10 +13913,10 @@
         <v>42</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>210</v>
@@ -13917,10 +13950,10 @@
         <v>42</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>210</v>
@@ -13954,10 +13987,10 @@
         <v>42</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>210</v>
@@ -13991,10 +14024,10 @@
         <v>42</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>210</v>
@@ -14028,10 +14061,10 @@
         <v>32</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E32" s="14" t="s">
         <v>210</v>
@@ -14060,35 +14093,35 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L32">
-    <cfRule type="expression" dxfId="400" priority="68">
+    <cfRule type="expression" dxfId="404" priority="68">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17 D12 A2:A15 D3:D6 A16:B16 D24:D27 A17:A32">
-    <cfRule type="expression" dxfId="399" priority="52">
+    <cfRule type="expression" dxfId="403" priority="52">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="398" priority="53">
+    <cfRule type="expression" dxfId="402" priority="53">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:L2 B21:E21 B17:C17 B12:C12 E12 B3:C6 E3:L4 E5:E6 E17:L17 G21:L21 F21:F23 F28:F32 B7:E11 B13:E15 F5:L15">
-    <cfRule type="expression" dxfId="397" priority="151">
+    <cfRule type="expression" dxfId="401" priority="151">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:L16">
-    <cfRule type="expression" dxfId="396" priority="11">
+    <cfRule type="expression" dxfId="400" priority="11">
       <formula>ISBLANK($F16)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:F20">
-    <cfRule type="expression" dxfId="395" priority="9">
+    <cfRule type="expression" dxfId="399" priority="9">
       <formula>ISBLANK($F18)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:C27 E24:F27 H24:L27">
-    <cfRule type="expression" dxfId="394" priority="5">
+    <cfRule type="expression" dxfId="398" priority="5">
       <formula>ISBLANK($F24)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14362,7 +14395,7 @@
         <v>32</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>177</v>
@@ -14473,7 +14506,7 @@
         <v>32</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>150</v>
@@ -14621,13 +14654,13 @@
         <v>32</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>3</v>
@@ -14658,13 +14691,13 @@
         <v>32</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>3</v>
@@ -14695,13 +14728,13 @@
         <v>32</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>3</v>
@@ -14769,13 +14802,13 @@
         <v>32</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>3</v>
@@ -14806,13 +14839,13 @@
         <v>32</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>3</v>
@@ -14843,13 +14876,13 @@
         <v>32</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>3</v>
@@ -14880,13 +14913,13 @@
         <v>32</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>3</v>
@@ -14917,10 +14950,10 @@
         <v>42</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>210</v>
@@ -14954,10 +14987,10 @@
         <v>42</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>210</v>
@@ -14991,10 +15024,10 @@
         <v>42</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>210</v>
@@ -15028,10 +15061,10 @@
         <v>42</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E25" s="14" t="s">
         <v>210</v>
@@ -15065,10 +15098,10 @@
         <v>32</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>210</v>
@@ -15097,73 +15130,73 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L15 G17:L26">
-    <cfRule type="expression" dxfId="377" priority="70">
+    <cfRule type="expression" dxfId="381" priority="70">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 D9 D3:D6 A2:A11 A12:B12 A13:A15 D18:D21 A17:A26">
-    <cfRule type="expression" dxfId="376" priority="51">
+    <cfRule type="expression" dxfId="380" priority="51">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="375" priority="52">
+    <cfRule type="expression" dxfId="379" priority="52">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:E7 B8:C11 E8:E11 B2:C6 E2:L4 E5:E6 F5:L11 E13:L13 B13:C13 B17:L17 F22:F26">
-    <cfRule type="expression" dxfId="374" priority="161">
+    <cfRule type="expression" dxfId="378" priority="161">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="373" priority="24">
+    <cfRule type="expression" dxfId="377" priority="24">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="expression" dxfId="372" priority="23">
+    <cfRule type="expression" dxfId="376" priority="23">
       <formula>ISBLANK($F8)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="371" priority="22">
+    <cfRule type="expression" dxfId="375" priority="22">
       <formula>ISBLANK($F11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="370" priority="21">
+    <cfRule type="expression" dxfId="374" priority="21">
       <formula>ISBLANK($F10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:L12">
-    <cfRule type="expression" dxfId="369" priority="16">
+    <cfRule type="expression" dxfId="373" priority="16">
       <formula>ISBLANK($F12)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:F15">
-    <cfRule type="expression" dxfId="368" priority="14">
+    <cfRule type="expression" dxfId="372" priority="14">
       <formula>ISBLANK($F14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C21 E18:F21 H18:L21">
-    <cfRule type="expression" dxfId="367" priority="10">
+    <cfRule type="expression" dxfId="371" priority="10">
       <formula>ISBLANK($F18)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16:L16">
-    <cfRule type="expression" dxfId="366" priority="4">
+    <cfRule type="expression" dxfId="370" priority="4">
       <formula>NOT((COLUMN(G16)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F16, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="expression" dxfId="365" priority="2">
+    <cfRule type="expression" dxfId="369" priority="2">
       <formula>ISBLANK($F16)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="364" priority="3">
+    <cfRule type="expression" dxfId="368" priority="3">
       <formula>NOT((COLUMN(A16)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F16, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="expression" dxfId="363" priority="1">
+    <cfRule type="expression" dxfId="367" priority="1">
       <formula>ISBLANK($F16)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15184,7 +15217,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -15251,7 +15284,7 @@
         <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>151</v>
@@ -15695,13 +15728,13 @@
         <v>32</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>3</v>
@@ -15732,13 +15765,13 @@
         <v>32</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>3</v>
@@ -15769,13 +15802,13 @@
         <v>32</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>3</v>
@@ -15806,13 +15839,13 @@
         <v>32</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>3</v>
@@ -15843,13 +15876,13 @@
         <v>32</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>3</v>
@@ -15880,13 +15913,13 @@
         <v>32</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>3</v>
@@ -15917,13 +15950,13 @@
         <v>32</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>3</v>
@@ -15954,10 +15987,10 @@
         <v>42</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>210</v>
@@ -15991,10 +16024,10 @@
         <v>42</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>210</v>
@@ -16028,10 +16061,10 @@
         <v>42</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>210</v>
@@ -16065,10 +16098,10 @@
         <v>42</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>210</v>
@@ -16097,50 +16130,50 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L24">
-    <cfRule type="expression" dxfId="346" priority="84">
+    <cfRule type="expression" dxfId="350" priority="84">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A11 D3:D7 A12:B12 D13 D17:D20 A13:A24">
-    <cfRule type="expression" dxfId="345" priority="62">
+    <cfRule type="expression" dxfId="349" priority="62">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="344" priority="63">
+    <cfRule type="expression" dxfId="348" priority="63">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:L2 B13:C13 E3:L4 E13:L13 F21:F24 B3:C9 E5:E9 B10:E11 F5:L11">
-    <cfRule type="expression" dxfId="343" priority="159">
+    <cfRule type="expression" dxfId="347" priority="159">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="342" priority="25">
+    <cfRule type="expression" dxfId="346" priority="25">
       <formula>ISBLANK($F9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="expression" dxfId="341" priority="23">
+    <cfRule type="expression" dxfId="345" priority="23">
       <formula>ISBLANK($F8)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:L12">
-    <cfRule type="expression" dxfId="340" priority="16">
+    <cfRule type="expression" dxfId="344" priority="16">
       <formula>ISBLANK($F12)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C20 E17:F20 H17:L20">
-    <cfRule type="expression" dxfId="339" priority="14">
+    <cfRule type="expression" dxfId="343" priority="14">
       <formula>ISBLANK($F17)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:F15">
-    <cfRule type="expression" dxfId="338" priority="5">
+    <cfRule type="expression" dxfId="342" priority="5">
       <formula>ISBLANK($F14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="expression" dxfId="337" priority="1">
+    <cfRule type="expression" dxfId="341" priority="1">
       <formula>ISBLANK($F16)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16162,7 +16195,7 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="C22" sqref="C22:O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16493,7 +16526,7 @@
         <v>45</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>175</v>
@@ -16567,7 +16600,7 @@
         <v>45</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>145</v>
@@ -16715,7 +16748,7 @@
         <v>32</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>148</v>
@@ -16826,13 +16859,13 @@
         <v>32</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>3</v>
@@ -16863,13 +16896,13 @@
         <v>32</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>3</v>
@@ -16900,13 +16933,13 @@
         <v>32</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>3</v>
@@ -16974,10 +17007,10 @@
         <v>32</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>220</v>
+        <v>314</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>214</v>
+        <v>315</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>211</v>
@@ -16986,7 +17019,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="14">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
@@ -16997,10 +17030,10 @@
         <v>0</v>
       </c>
       <c r="N22" s="14">
-        <v>10000</v>
+        <v>72</v>
       </c>
       <c r="O22" s="14">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -17014,10 +17047,10 @@
         <v>202</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F23" s="11" t="s">
         <v>3</v>
@@ -17048,13 +17081,13 @@
         <v>32</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F24" s="11" t="s">
         <v>3</v>
@@ -17085,13 +17118,13 @@
         <v>32</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>3</v>
@@ -17122,13 +17155,13 @@
         <v>32</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>3</v>
@@ -17159,13 +17192,13 @@
         <v>32</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>3</v>
@@ -17196,10 +17229,10 @@
         <v>42</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>210</v>
@@ -17233,10 +17266,10 @@
         <v>42</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>210</v>
@@ -17270,10 +17303,10 @@
         <v>42</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>210</v>
@@ -17307,10 +17340,10 @@
         <v>42</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>210</v>
@@ -17344,10 +17377,10 @@
         <v>32</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E32" s="14" t="s">
         <v>210</v>
@@ -17374,37 +17407,47 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:L32">
-    <cfRule type="expression" dxfId="319" priority="6">
+  <conditionalFormatting sqref="G2:L21 G23:L32">
+    <cfRule type="expression" dxfId="323" priority="8">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17 D12 A2:A15 D3:D6 A16:B16 D24:D27 A17:A32">
-    <cfRule type="expression" dxfId="318" priority="4">
+    <cfRule type="expression" dxfId="322" priority="6">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="317" priority="5">
+    <cfRule type="expression" dxfId="321" priority="7">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:L2 B21:E21 B17:C17 B12:C12 E12 B3:C6 E3:L4 E5:E6 E17:L17 G21:L21 F21:F23 F28:F32 B7:E11 B13:E15 F5:L15">
-    <cfRule type="expression" dxfId="316" priority="7">
+  <conditionalFormatting sqref="B2:L2 B17:C17 B12:C12 E12 B3:C6 E3:L4 E5:E6 E17:L17 B21:L21 F28:F32 B7:E11 B13:E15 F5:L15 F23">
+    <cfRule type="expression" dxfId="320" priority="9">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:L16">
-    <cfRule type="expression" dxfId="315" priority="3">
+    <cfRule type="expression" dxfId="319" priority="5">
       <formula>ISBLANK($F16)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:F20">
-    <cfRule type="expression" dxfId="314" priority="2">
+    <cfRule type="expression" dxfId="318" priority="4">
       <formula>ISBLANK($F18)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:C27 E24:F27 H24:L27">
-    <cfRule type="expression" dxfId="313" priority="1">
+    <cfRule type="expression" dxfId="317" priority="3">
       <formula>ISBLANK($F24)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G22:L22">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>NOT((COLUMN(G22)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F22, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>ISBLANK($F22)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -17423,8 +17466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87277472-6F92-4209-B3A9-C72FCC829F3A}">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17718,13 +17761,13 @@
         <v>45</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>3</v>
@@ -17755,13 +17798,13 @@
         <v>45</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>3</v>
@@ -17792,13 +17835,13 @@
         <v>45</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>3</v>
@@ -17940,7 +17983,7 @@
         <v>32</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>148</v>
@@ -18051,13 +18094,13 @@
         <v>32</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>3</v>
@@ -18088,10 +18131,10 @@
         <v>32</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>220</v>
+        <v>314</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>214</v>
+        <v>315</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>211</v>
@@ -18100,7 +18143,7 @@
         <v>3</v>
       </c>
       <c r="G18" s="14">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
@@ -18111,10 +18154,10 @@
         <v>0</v>
       </c>
       <c r="N18" s="14">
-        <v>10000</v>
+        <v>72</v>
       </c>
       <c r="O18" s="14">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -18125,13 +18168,13 @@
         <v>32</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>3</v>
@@ -18162,13 +18205,13 @@
         <v>32</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>3</v>
@@ -18202,10 +18245,10 @@
         <v>202</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>3</v>
@@ -18236,13 +18279,13 @@
         <v>32</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>3</v>
@@ -18273,13 +18316,13 @@
         <v>32</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F23" s="11" t="s">
         <v>3</v>
@@ -18310,13 +18353,13 @@
         <v>32</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F24" s="11" t="s">
         <v>3</v>
@@ -18347,13 +18390,13 @@
         <v>32</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>3</v>
@@ -18384,13 +18427,13 @@
         <v>32</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>3</v>
@@ -18421,10 +18464,10 @@
         <v>42</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>210</v>
@@ -18458,10 +18501,10 @@
         <v>42</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>210</v>
@@ -18495,10 +18538,10 @@
         <v>42</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>210</v>
@@ -18532,10 +18575,10 @@
         <v>42</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>210</v>
@@ -18572,7 +18615,7 @@
         <v>203</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>34</v>
@@ -18606,10 +18649,10 @@
         <v>32</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>180</v>
@@ -18643,10 +18686,10 @@
         <v>32</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>183</v>
@@ -18680,10 +18723,10 @@
         <v>32</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E34" s="14" t="s">
         <v>210</v>
@@ -18711,47 +18754,57 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G2:L34">
-    <cfRule type="expression" dxfId="296" priority="10">
+  <conditionalFormatting sqref="G2:L17 G19:L34">
+    <cfRule type="expression" dxfId="300" priority="12">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15 D11 D3:D6 D31 A27:A34 A2:A21 G11:L16 F11:F21 B12:E14">
-    <cfRule type="expression" dxfId="295" priority="11">
+  <conditionalFormatting sqref="D15 D11 D3:D6 D31 A27:A34 A2:A21 G11:L16 F11:F17 B12:E14 F19:F21">
+    <cfRule type="expression" dxfId="299" priority="13">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:L10 F27">
-    <cfRule type="expression" dxfId="294" priority="12">
+    <cfRule type="expression" dxfId="298" priority="14">
       <formula>ISBLANK($F7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:L2 B16:E16 B15:C15 E15 B11:C11 E11 B3:C6 E3:L6">
-    <cfRule type="expression" dxfId="293" priority="13">
+    <cfRule type="expression" dxfId="297" priority="15">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:L33">
-    <cfRule type="expression" dxfId="292" priority="9">
+    <cfRule type="expression" dxfId="296" priority="11">
       <formula>ISBLANK($F32)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D26 A22:A26">
-    <cfRule type="expression" dxfId="291" priority="5">
+    <cfRule type="expression" dxfId="295" priority="7">
       <formula>ISBLANK($F22)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="290" priority="6">
+    <cfRule type="expression" dxfId="294" priority="8">
       <formula>NOT((COLUMN(A22)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F22, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="expression" dxfId="289" priority="14">
+    <cfRule type="expression" dxfId="293" priority="16">
       <formula>ISBLANK($F22)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C26 E23:F26 H23:L26">
-    <cfRule type="expression" dxfId="288" priority="1">
+    <cfRule type="expression" dxfId="292" priority="3">
       <formula>ISBLANK($F23)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18:L18">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>NOT((COLUMN(G18)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F18, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>ISBLANK($F18)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>